<commit_message>
South Korea label on top
</commit_message>
<xml_diff>
--- a/Codes_Masterlist.xlsx
+++ b/Codes_Masterlist.xlsx
@@ -18241,7 +18241,7 @@
         <v>719</v>
       </c>
       <c r="C197" t="s">
-        <v>720</v>
+        <v>727</v>
       </c>
       <c r="D197" t="s">
         <v>39</v>
@@ -18309,7 +18309,7 @@
         <v>719</v>
       </c>
       <c r="C198" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="D198" t="s">
         <v>39</v>
@@ -18377,7 +18377,7 @@
         <v>719</v>
       </c>
       <c r="C199" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="D199" t="s">
         <v>39</v>
@@ -18445,7 +18445,7 @@
         <v>719</v>
       </c>
       <c r="C200" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="D200" t="s">
         <v>39</v>
@@ -18513,7 +18513,7 @@
         <v>719</v>
       </c>
       <c r="C201" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="D201" t="s">
         <v>39</v>
@@ -18581,7 +18581,7 @@
         <v>719</v>
       </c>
       <c r="C202" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="D202" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
Put Spain label on top for ESP
</commit_message>
<xml_diff>
--- a/Codes_Masterlist.xlsx
+++ b/Codes_Masterlist.xlsx
@@ -12632,7 +12632,7 @@
         <v>438</v>
       </c>
       <c r="C115" t="s">
-        <v>1469</v>
+        <v>439</v>
       </c>
       <c r="D115" t="s">
         <v>66</v>
@@ -12703,7 +12703,7 @@
         <v>438</v>
       </c>
       <c r="C116" t="s">
-        <v>439</v>
+        <v>1469</v>
       </c>
       <c r="D116" t="s">
         <v>66</v>

</xml_diff>

<commit_message>
Label Portugal on top for PRT
</commit_message>
<xml_diff>
--- a/Codes_Masterlist.xlsx
+++ b/Codes_Masterlist.xlsx
@@ -24656,7 +24656,7 @@
         <v>1050</v>
       </c>
       <c r="C292" t="s">
-        <v>1479</v>
+        <v>1051</v>
       </c>
       <c r="D292" t="s">
         <v>66</v>
@@ -24727,7 +24727,7 @@
         <v>1050</v>
       </c>
       <c r="C293" t="s">
-        <v>1478</v>
+        <v>1479</v>
       </c>
       <c r="D293" t="s">
         <v>66</v>
@@ -24798,7 +24798,7 @@
         <v>1050</v>
       </c>
       <c r="C294" t="s">
-        <v>1051</v>
+        <v>1478</v>
       </c>
       <c r="D294" t="s">
         <v>66</v>

</xml_diff>

<commit_message>
Change order of labels
</commit_message>
<xml_diff>
--- a/Codes_Masterlist.xlsx
+++ b/Codes_Masterlist.xlsx
@@ -11437,7 +11437,7 @@
         <v>368</v>
       </c>
       <c r="C98" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="D98" t="s">
         <v>27</v>
@@ -11508,7 +11508,7 @@
         <v>368</v>
       </c>
       <c r="C99" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="D99" t="s">
         <v>27</v>
@@ -13395,7 +13395,7 @@
         <v>475</v>
       </c>
       <c r="C126" t="s">
-        <v>476</v>
+        <v>480</v>
       </c>
       <c r="D126" t="s">
         <v>66</v>
@@ -13460,7 +13460,7 @@
         <v>475</v>
       </c>
       <c r="C127" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="D127" t="s">
         <v>66</v>
@@ -13525,7 +13525,7 @@
         <v>475</v>
       </c>
       <c r="C128" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D128" t="s">
         <v>66</v>
@@ -15382,7 +15382,7 @@
         <v>578</v>
       </c>
       <c r="C155" t="s">
-        <v>579</v>
+        <v>584</v>
       </c>
       <c r="D155" t="s">
         <v>39</v>
@@ -15450,7 +15450,7 @@
         <v>578</v>
       </c>
       <c r="C156" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="D156" t="s">
         <v>39</v>
@@ -15518,7 +15518,7 @@
         <v>578</v>
       </c>
       <c r="C157" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="D157" t="s">
         <v>39</v>
@@ -15586,7 +15586,7 @@
         <v>578</v>
       </c>
       <c r="C158" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="D158" t="s">
         <v>39</v>
@@ -19908,7 +19908,7 @@
         <v>799</v>
       </c>
       <c r="C222" t="s">
-        <v>800</v>
+        <v>805</v>
       </c>
       <c r="D222" t="s">
         <v>39</v>
@@ -19973,7 +19973,7 @@
         <v>799</v>
       </c>
       <c r="C223" t="s">
-        <v>803</v>
+        <v>800</v>
       </c>
       <c r="D223" t="s">
         <v>39</v>
@@ -20038,7 +20038,7 @@
         <v>799</v>
       </c>
       <c r="C224" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="D224" t="s">
         <v>39</v>
@@ -20103,7 +20103,7 @@
         <v>799</v>
       </c>
       <c r="C225" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="D225" t="s">
         <v>39</v>
@@ -22782,7 +22782,7 @@
         <v>935</v>
       </c>
       <c r="C264" t="s">
-        <v>936</v>
+        <v>939</v>
       </c>
       <c r="D264" t="s">
         <v>112</v>
@@ -22847,7 +22847,7 @@
         <v>935</v>
       </c>
       <c r="C265" t="s">
-        <v>939</v>
+        <v>936</v>
       </c>
       <c r="D265" t="s">
         <v>112</v>
@@ -30098,7 +30098,7 @@
         <v>1278</v>
       </c>
       <c r="C373" t="s">
-        <v>1485</v>
+        <v>1279</v>
       </c>
       <c r="D373" t="s">
         <v>27</v>
@@ -30172,7 +30172,7 @@
         <v>1278</v>
       </c>
       <c r="C374" t="s">
-        <v>1484</v>
+        <v>1485</v>
       </c>
       <c r="D374" t="s">
         <v>27</v>
@@ -30246,7 +30246,7 @@
         <v>1278</v>
       </c>
       <c r="C375" t="s">
-        <v>1279</v>
+        <v>1484</v>
       </c>
       <c r="D375" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
Put St Kitts and Nevis label on top for KNA
</commit_message>
<xml_diff>
--- a/Codes_Masterlist.xlsx
+++ b/Codes_Masterlist.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\boxsync\alepissier\PhD\Software\Codes-Masterlist\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alice\Box Sync\PhD\Software\Codes-Masterlist\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81AB7DD3-34C6-4868-87C7-1EE26D553217}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31905" yWindow="-90" windowWidth="16980" windowHeight="10080"/>
+    <workbookView xWindow="31910" yWindow="-90" windowWidth="16980" windowHeight="10080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Codes" sheetId="1" r:id="rId1"/>
@@ -4499,7 +4500,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -4833,19 +4834,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y429"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="3" max="3" width="44.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="22" width="9.140625" customWidth="1"/>
-    <col min="23" max="23" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="22" width="9.1328125" customWidth="1"/>
+    <col min="23" max="23" width="17.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4922,7 +4923,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -4993,7 +4994,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -5064,7 +5065,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -5135,7 +5136,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>48</v>
       </c>
@@ -5209,7 +5210,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>58</v>
       </c>
@@ -5271,7 +5272,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
         <v>58</v>
       </c>
@@ -5333,7 +5334,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
         <v>63</v>
       </c>
@@ -5389,7 +5390,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
         <v>71</v>
       </c>
@@ -5457,7 +5458,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
         <v>79</v>
       </c>
@@ -5522,7 +5523,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
         <v>84</v>
       </c>
@@ -5545,7 +5546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
         <v>84</v>
       </c>
@@ -5568,7 +5569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A13" t="s">
         <v>88</v>
       </c>
@@ -5636,7 +5637,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A14" t="s">
         <v>88</v>
       </c>
@@ -5704,7 +5705,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A15" t="s">
         <v>88</v>
       </c>
@@ -5772,7 +5773,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A16" t="s">
         <v>97</v>
       </c>
@@ -5846,7 +5847,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A17" t="s">
         <v>103</v>
       </c>
@@ -5914,7 +5915,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A18" t="s">
         <v>103</v>
       </c>
@@ -5982,7 +5983,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A19" t="s">
         <v>109</v>
       </c>
@@ -6047,7 +6048,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A20" t="s">
         <v>117</v>
       </c>
@@ -6088,7 +6089,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A21" t="s">
         <v>117</v>
       </c>
@@ -6129,7 +6130,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A22" t="s">
         <v>122</v>
       </c>
@@ -6191,7 +6192,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A23" t="s">
         <v>122</v>
       </c>
@@ -6253,7 +6254,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A24" t="s">
         <v>128</v>
       </c>
@@ -6327,7 +6328,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A25" t="s">
         <v>128</v>
       </c>
@@ -6401,7 +6402,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A26" t="s">
         <v>128</v>
       </c>
@@ -6475,7 +6476,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A27" t="s">
         <v>128</v>
       </c>
@@ -6549,7 +6550,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A28" t="s">
         <v>134</v>
       </c>
@@ -6617,7 +6618,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A29" t="s">
         <v>140</v>
       </c>
@@ -6688,7 +6689,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A30" t="s">
         <v>147</v>
       </c>
@@ -6756,7 +6757,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A31" t="s">
         <v>147</v>
       </c>
@@ -6824,7 +6825,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A32" t="s">
         <v>153</v>
       </c>
@@ -6901,7 +6902,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A33" t="s">
         <v>158</v>
       </c>
@@ -6972,7 +6973,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A34" t="s">
         <v>163</v>
       </c>
@@ -7049,7 +7050,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A35" t="s">
         <v>169</v>
       </c>
@@ -7105,7 +7106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A36" t="s">
         <v>169</v>
       </c>
@@ -7161,7 +7162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A37" t="s">
         <v>169</v>
       </c>
@@ -7217,7 +7218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A38" t="s">
         <v>169</v>
       </c>
@@ -7273,7 +7274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A39" t="s">
         <v>169</v>
       </c>
@@ -7329,7 +7330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A40" t="s">
         <v>173</v>
       </c>
@@ -7406,7 +7407,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A41" t="s">
         <v>178</v>
       </c>
@@ -7474,7 +7475,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A42" t="s">
         <v>183</v>
       </c>
@@ -7542,7 +7543,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A43" t="s">
         <v>189</v>
       </c>
@@ -7610,7 +7611,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A44" t="s">
         <v>189</v>
       </c>
@@ -7678,7 +7679,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A45" t="s">
         <v>195</v>
       </c>
@@ -7752,7 +7753,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A46" t="s">
         <v>195</v>
       </c>
@@ -7826,7 +7827,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A47" t="s">
         <v>201</v>
       </c>
@@ -7894,7 +7895,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A48" t="s">
         <v>201</v>
       </c>
@@ -7962,7 +7963,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A49" t="s">
         <v>207</v>
       </c>
@@ -8024,7 +8025,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A50" t="s">
         <v>207</v>
       </c>
@@ -8086,7 +8087,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A51" t="s">
         <v>207</v>
       </c>
@@ -8148,7 +8149,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A52" t="s">
         <v>212</v>
       </c>
@@ -8216,7 +8217,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A53" t="s">
         <v>217</v>
       </c>
@@ -8290,7 +8291,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A54" t="s">
         <v>223</v>
       </c>
@@ -8355,7 +8356,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A55" t="s">
         <v>230</v>
       </c>
@@ -8432,7 +8433,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A56" t="s">
         <v>230</v>
       </c>
@@ -8509,7 +8510,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A57" t="s">
         <v>236</v>
       </c>
@@ -8583,7 +8584,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A58" t="s">
         <v>241</v>
       </c>
@@ -8657,7 +8658,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A59" t="s">
         <v>246</v>
       </c>
@@ -8725,7 +8726,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A60" t="s">
         <v>246</v>
       </c>
@@ -8793,7 +8794,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A61" t="s">
         <v>253</v>
       </c>
@@ -8861,7 +8862,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A62" t="s">
         <v>258</v>
       </c>
@@ -8917,7 +8918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A63" t="s">
         <v>261</v>
       </c>
@@ -8991,7 +8992,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="64" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A64" t="s">
         <v>267</v>
       </c>
@@ -9068,7 +9069,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="65" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A65" t="s">
         <v>267</v>
       </c>
@@ -9145,7 +9146,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="66" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A66" t="s">
         <v>273</v>
       </c>
@@ -9213,7 +9214,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="67" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A67" t="s">
         <v>278</v>
       </c>
@@ -9263,7 +9264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A68" t="s">
         <v>278</v>
       </c>
@@ -9313,7 +9314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A69" t="s">
         <v>281</v>
       </c>
@@ -9381,7 +9382,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="70" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A70" t="s">
         <v>286</v>
       </c>
@@ -9455,7 +9456,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="71" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A71" t="s">
         <v>291</v>
       </c>
@@ -9523,7 +9524,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="72" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A72" t="s">
         <v>291</v>
       </c>
@@ -9591,7 +9592,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="73" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A73" t="s">
         <v>298</v>
       </c>
@@ -9668,7 +9669,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="74" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A74" t="s">
         <v>298</v>
       </c>
@@ -9745,7 +9746,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="75" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A75" t="s">
         <v>298</v>
       </c>
@@ -9822,7 +9823,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="76" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A76" t="s">
         <v>304</v>
       </c>
@@ -9899,7 +9900,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="77" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A77" t="s">
         <v>310</v>
       </c>
@@ -9976,7 +9977,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="78" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A78" t="s">
         <v>310</v>
       </c>
@@ -10053,7 +10054,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="79" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A79" t="s">
         <v>310</v>
       </c>
@@ -10130,7 +10131,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="80" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A80" t="s">
         <v>310</v>
       </c>
@@ -10207,7 +10208,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="81" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A81" t="s">
         <v>310</v>
       </c>
@@ -10284,7 +10285,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="82" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A82" t="s">
         <v>319</v>
       </c>
@@ -10361,7 +10362,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="83" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A83" t="s">
         <v>319</v>
       </c>
@@ -10438,7 +10439,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="84" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A84" t="s">
         <v>319</v>
       </c>
@@ -10515,7 +10516,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="85" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A85" t="s">
         <v>319</v>
       </c>
@@ -10592,7 +10593,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="86" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A86" t="s">
         <v>326</v>
       </c>
@@ -10648,7 +10649,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="87" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A87" t="s">
         <v>331</v>
       </c>
@@ -10722,7 +10723,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="88" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A88" t="s">
         <v>336</v>
       </c>
@@ -10799,7 +10800,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="89" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A89" t="s">
         <v>341</v>
       </c>
@@ -10873,7 +10874,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="90" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A90" t="s">
         <v>341</v>
       </c>
@@ -10947,7 +10948,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="91" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A91" t="s">
         <v>341</v>
       </c>
@@ -11021,7 +11022,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="92" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A92" t="s">
         <v>348</v>
       </c>
@@ -11095,7 +11096,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="93" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A93" t="s">
         <v>353</v>
       </c>
@@ -11166,7 +11167,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="94" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A94" t="s">
         <v>358</v>
       </c>
@@ -11237,7 +11238,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="95" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A95" t="s">
         <v>358</v>
       </c>
@@ -11308,7 +11309,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="96" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A96" t="s">
         <v>358</v>
       </c>
@@ -11379,7 +11380,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="97" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A97" t="s">
         <v>364</v>
       </c>
@@ -11429,7 +11430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A98" t="s">
         <v>367</v>
       </c>
@@ -11500,7 +11501,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="99" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A99" t="s">
         <v>367</v>
       </c>
@@ -11571,7 +11572,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="100" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A100" t="s">
         <v>373</v>
       </c>
@@ -11642,7 +11643,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="101" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A101" t="s">
         <v>378</v>
       </c>
@@ -11710,7 +11711,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="102" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A102" t="s">
         <v>378</v>
       </c>
@@ -11778,7 +11779,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="103" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A103" t="s">
         <v>384</v>
       </c>
@@ -11849,7 +11850,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="104" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A104" t="s">
         <v>389</v>
       </c>
@@ -11923,7 +11924,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="105" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A105" t="s">
         <v>394</v>
       </c>
@@ -11997,7 +11998,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="106" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A106" t="s">
         <v>399</v>
       </c>
@@ -12065,7 +12066,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="107" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A107" t="s">
         <v>404</v>
       </c>
@@ -12139,7 +12140,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="108" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A108" t="s">
         <v>404</v>
       </c>
@@ -12213,7 +12214,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="109" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A109" t="s">
         <v>410</v>
       </c>
@@ -12281,7 +12282,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="110" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A110" t="s">
         <v>416</v>
       </c>
@@ -12355,7 +12356,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="111" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A111" t="s">
         <v>421</v>
       </c>
@@ -12423,7 +12424,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="112" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A112" t="s">
         <v>421</v>
       </c>
@@ -12491,7 +12492,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="113" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A113" t="s">
         <v>427</v>
       </c>
@@ -12568,7 +12569,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="114" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A114" t="s">
         <v>432</v>
       </c>
@@ -12624,7 +12625,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="115" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A115" t="s">
         <v>437</v>
       </c>
@@ -12695,7 +12696,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="116" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A116" t="s">
         <v>437</v>
       </c>
@@ -12766,7 +12767,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="117" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A117" t="s">
         <v>442</v>
       </c>
@@ -12837,7 +12838,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="118" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A118" t="s">
         <v>447</v>
       </c>
@@ -12914,7 +12915,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="119" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A119" t="s">
         <v>447</v>
       </c>
@@ -12991,7 +12992,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="120" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A120" t="s">
         <v>452</v>
       </c>
@@ -13062,7 +13063,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="121" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A121" t="s">
         <v>457</v>
       </c>
@@ -13130,7 +13131,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="122" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A122" t="s">
         <v>463</v>
       </c>
@@ -13192,7 +13193,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="123" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A123" t="s">
         <v>463</v>
       </c>
@@ -13254,7 +13255,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="124" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A124" t="s">
         <v>463</v>
       </c>
@@ -13316,7 +13317,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="125" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A125" t="s">
         <v>469</v>
       </c>
@@ -13387,7 +13388,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="126" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A126" t="s">
         <v>474</v>
       </c>
@@ -13452,7 +13453,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="127" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A127" t="s">
         <v>474</v>
       </c>
@@ -13517,7 +13518,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="128" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A128" t="s">
         <v>474</v>
       </c>
@@ -13582,7 +13583,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="129" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A129" t="s">
         <v>481</v>
       </c>
@@ -13650,7 +13651,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="130" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A130" t="s">
         <v>481</v>
       </c>
@@ -13718,7 +13719,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="131" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A131" t="s">
         <v>481</v>
       </c>
@@ -13786,7 +13787,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="132" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A132" t="s">
         <v>481</v>
       </c>
@@ -13854,7 +13855,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="133" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A133" t="s">
         <v>489</v>
       </c>
@@ -13928,7 +13929,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="134" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A134" t="s">
         <v>494</v>
       </c>
@@ -13996,7 +13997,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="135" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A135" t="s">
         <v>494</v>
       </c>
@@ -14064,7 +14065,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="136" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A136" t="s">
         <v>494</v>
       </c>
@@ -14132,7 +14133,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="137" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A137" t="s">
         <v>500</v>
       </c>
@@ -14200,7 +14201,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="138" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A138" t="s">
         <v>505</v>
       </c>
@@ -14262,7 +14263,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="139" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A139" t="s">
         <v>511</v>
       </c>
@@ -14339,7 +14340,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="140" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A140" t="s">
         <v>516</v>
       </c>
@@ -14398,7 +14399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A141" t="s">
         <v>519</v>
       </c>
@@ -14475,7 +14476,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="142" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A142" t="s">
         <v>524</v>
       </c>
@@ -14531,7 +14532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A143" t="s">
         <v>527</v>
       </c>
@@ -14608,7 +14609,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="144" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A144" t="s">
         <v>527</v>
       </c>
@@ -14685,7 +14686,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="145" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A145" t="s">
         <v>533</v>
       </c>
@@ -14762,7 +14763,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="146" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A146" t="s">
         <v>538</v>
       </c>
@@ -14836,7 +14837,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="147" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A147" t="s">
         <v>543</v>
       </c>
@@ -14907,7 +14908,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="148" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A148" t="s">
         <v>548</v>
       </c>
@@ -14981,7 +14982,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="149" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A149" t="s">
         <v>553</v>
       </c>
@@ -15046,7 +15047,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="150" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A150" t="s">
         <v>558</v>
       </c>
@@ -15120,7 +15121,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="151" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A151" t="s">
         <v>563</v>
       </c>
@@ -15176,7 +15177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A152" t="s">
         <v>563</v>
       </c>
@@ -15232,7 +15233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A153" t="s">
         <v>567</v>
       </c>
@@ -15297,7 +15298,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="154" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A154" t="s">
         <v>572</v>
       </c>
@@ -15374,7 +15375,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="155" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A155" t="s">
         <v>577</v>
       </c>
@@ -15442,7 +15443,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="156" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A156" t="s">
         <v>577</v>
       </c>
@@ -15510,7 +15511,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="157" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A157" t="s">
         <v>577</v>
       </c>
@@ -15578,7 +15579,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="158" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A158" t="s">
         <v>577</v>
       </c>
@@ -15646,7 +15647,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="159" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A159" t="s">
         <v>577</v>
       </c>
@@ -15714,7 +15715,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="160" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A160" t="s">
         <v>577</v>
       </c>
@@ -15782,7 +15783,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="161" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A161" t="s">
         <v>577</v>
       </c>
@@ -15850,7 +15851,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="162" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A162" t="s">
         <v>587</v>
       </c>
@@ -15906,7 +15907,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="163" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A163" t="s">
         <v>587</v>
       </c>
@@ -15962,7 +15963,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="164" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A164" t="s">
         <v>587</v>
       </c>
@@ -16018,7 +16019,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="165" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A165" t="s">
         <v>592</v>
       </c>
@@ -16095,7 +16096,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="166" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A166" t="s">
         <v>597</v>
       </c>
@@ -16163,7 +16164,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="167" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A167" t="s">
         <v>602</v>
       </c>
@@ -16240,7 +16241,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="168" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A168" t="s">
         <v>607</v>
       </c>
@@ -16308,7 +16309,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="169" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A169" t="s">
         <v>612</v>
       </c>
@@ -16376,7 +16377,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="170" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A170" t="s">
         <v>617</v>
       </c>
@@ -16441,7 +16442,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="171" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A171" t="s">
         <v>622</v>
       </c>
@@ -16509,7 +16510,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="172" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A172" t="s">
         <v>627</v>
       </c>
@@ -16571,7 +16572,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="173" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A173" t="s">
         <v>627</v>
       </c>
@@ -16633,7 +16634,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="174" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A174" t="s">
         <v>632</v>
       </c>
@@ -16704,7 +16705,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="175" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A175" t="s">
         <v>637</v>
       </c>
@@ -16772,7 +16773,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="176" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A176" t="s">
         <v>637</v>
       </c>
@@ -16840,7 +16841,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="177" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A177" t="s">
         <v>637</v>
       </c>
@@ -16908,7 +16909,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="178" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A178" t="s">
         <v>637</v>
       </c>
@@ -16976,7 +16977,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="179" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A179" t="s">
         <v>645</v>
       </c>
@@ -17044,7 +17045,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="180" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A180" t="s">
         <v>650</v>
       </c>
@@ -17112,7 +17113,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="181" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A181" t="s">
         <v>655</v>
       </c>
@@ -17180,7 +17181,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="182" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A182" t="s">
         <v>660</v>
       </c>
@@ -17251,7 +17252,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="183" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A183" t="s">
         <v>665</v>
       </c>
@@ -17325,7 +17326,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="184" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A184" t="s">
         <v>670</v>
       </c>
@@ -17387,7 +17388,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="185" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A185" t="s">
         <v>675</v>
       </c>
@@ -17455,7 +17456,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="186" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A186" t="s">
         <v>680</v>
       </c>
@@ -17523,7 +17524,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="187" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A187" t="s">
         <v>685</v>
       </c>
@@ -17591,7 +17592,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="188" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A188" t="s">
         <v>691</v>
       </c>
@@ -17665,7 +17666,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="189" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A189" t="s">
         <v>696</v>
       </c>
@@ -17733,7 +17734,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="190" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A190" t="s">
         <v>696</v>
       </c>
@@ -17801,7 +17802,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="191" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A191" t="s">
         <v>702</v>
       </c>
@@ -17869,7 +17870,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="192" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A192" t="s">
         <v>707</v>
       </c>
@@ -17937,7 +17938,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="193" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A193" t="s">
         <v>712</v>
       </c>
@@ -17945,7 +17946,7 @@
         <v>713</v>
       </c>
       <c r="C193" t="s">
-        <v>1473</v>
+        <v>717</v>
       </c>
       <c r="D193" t="s">
         <v>27</v>
@@ -18002,7 +18003,7 @@
         <v>0</v>
       </c>
       <c r="W193">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X193" t="s">
         <v>715</v>
@@ -18011,7 +18012,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="194" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A194" t="s">
         <v>712</v>
       </c>
@@ -18019,7 +18020,7 @@
         <v>713</v>
       </c>
       <c r="C194" t="s">
-        <v>1474</v>
+        <v>1473</v>
       </c>
       <c r="D194" t="s">
         <v>27</v>
@@ -18076,7 +18077,7 @@
         <v>0</v>
       </c>
       <c r="W194">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X194" t="s">
         <v>715</v>
@@ -18085,7 +18086,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="195" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A195" t="s">
         <v>712</v>
       </c>
@@ -18093,7 +18094,7 @@
         <v>713</v>
       </c>
       <c r="C195" t="s">
-        <v>714</v>
+        <v>1474</v>
       </c>
       <c r="D195" t="s">
         <v>27</v>
@@ -18159,7 +18160,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="196" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A196" t="s">
         <v>712</v>
       </c>
@@ -18167,7 +18168,7 @@
         <v>713</v>
       </c>
       <c r="C196" t="s">
-        <v>717</v>
+        <v>714</v>
       </c>
       <c r="D196" t="s">
         <v>27</v>
@@ -18233,7 +18234,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="197" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A197" t="s">
         <v>718</v>
       </c>
@@ -18301,7 +18302,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="198" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A198" t="s">
         <v>718</v>
       </c>
@@ -18369,7 +18370,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="199" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A199" t="s">
         <v>718</v>
       </c>
@@ -18437,7 +18438,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="200" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A200" t="s">
         <v>718</v>
       </c>
@@ -18505,7 +18506,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="201" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A201" t="s">
         <v>718</v>
       </c>
@@ -18573,7 +18574,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="202" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A202" t="s">
         <v>718</v>
       </c>
@@ -18641,7 +18642,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="203" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A203" t="s">
         <v>728</v>
       </c>
@@ -18676,7 +18677,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="204" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A204" t="s">
         <v>728</v>
       </c>
@@ -18711,7 +18712,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="205" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A205" t="s">
         <v>733</v>
       </c>
@@ -18779,7 +18780,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="206" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A206" t="s">
         <v>738</v>
       </c>
@@ -18847,7 +18848,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="207" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A207" t="s">
         <v>738</v>
       </c>
@@ -18915,7 +18916,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="208" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A208" t="s">
         <v>738</v>
       </c>
@@ -18983,7 +18984,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="209" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A209" t="s">
         <v>738</v>
       </c>
@@ -19051,7 +19052,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="210" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A210" t="s">
         <v>746</v>
       </c>
@@ -19119,7 +19120,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="211" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A211" t="s">
         <v>751</v>
       </c>
@@ -19196,7 +19197,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="212" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A212" t="s">
         <v>756</v>
       </c>
@@ -19264,7 +19265,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="213" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A213" t="s">
         <v>756</v>
       </c>
@@ -19332,7 +19333,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="214" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A214" t="s">
         <v>762</v>
       </c>
@@ -19406,7 +19407,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="215" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A215" t="s">
         <v>762</v>
       </c>
@@ -19480,7 +19481,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="216" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A216" t="s">
         <v>768</v>
       </c>
@@ -19545,7 +19546,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="217" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A217" t="s">
         <v>773</v>
       </c>
@@ -19613,7 +19614,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="218" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A218" t="s">
         <v>778</v>
       </c>
@@ -19687,7 +19688,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="219" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A219" t="s">
         <v>783</v>
       </c>
@@ -19758,7 +19759,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="220" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A220" t="s">
         <v>788</v>
       </c>
@@ -19829,7 +19830,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="221" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A221" t="s">
         <v>793</v>
       </c>
@@ -19900,7 +19901,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="222" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A222" t="s">
         <v>798</v>
       </c>
@@ -19965,7 +19966,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="223" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A223" t="s">
         <v>798</v>
       </c>
@@ -20030,7 +20031,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="224" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A224" t="s">
         <v>798</v>
       </c>
@@ -20095,7 +20096,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="225" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A225" t="s">
         <v>798</v>
       </c>
@@ -20160,7 +20161,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="226" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A226" t="s">
         <v>798</v>
       </c>
@@ -20225,7 +20226,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="227" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A227" t="s">
         <v>798</v>
       </c>
@@ -20290,7 +20291,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="228" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A228" t="s">
         <v>808</v>
       </c>
@@ -20361,7 +20362,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="229" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A229" t="s">
         <v>808</v>
       </c>
@@ -20432,7 +20433,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="230" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A230" t="s">
         <v>808</v>
       </c>
@@ -20503,7 +20504,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="231" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A231" t="s">
         <v>814</v>
       </c>
@@ -20571,7 +20572,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="232" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A232" t="s">
         <v>819</v>
       </c>
@@ -20636,7 +20637,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="233" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A233" t="s">
         <v>824</v>
       </c>
@@ -20704,7 +20705,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="234" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A234" t="s">
         <v>824</v>
       </c>
@@ -20772,7 +20773,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="235" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A235" t="s">
         <v>824</v>
       </c>
@@ -20840,7 +20841,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="236" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A236" t="s">
         <v>831</v>
       </c>
@@ -20917,7 +20918,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="237" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A237" t="s">
         <v>836</v>
       </c>
@@ -20985,7 +20986,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="238" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A238" t="s">
         <v>841</v>
       </c>
@@ -21059,7 +21060,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="239" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A239" t="s">
         <v>846</v>
       </c>
@@ -21127,7 +21128,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="240" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A240" t="s">
         <v>846</v>
       </c>
@@ -21195,7 +21196,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="241" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A241" t="s">
         <v>852</v>
       </c>
@@ -21263,7 +21264,7 @@
         <v>856</v>
       </c>
     </row>
-    <row r="242" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A242" t="s">
         <v>852</v>
       </c>
@@ -21331,7 +21332,7 @@
         <v>856</v>
       </c>
     </row>
-    <row r="243" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A243" t="s">
         <v>852</v>
       </c>
@@ -21399,7 +21400,7 @@
         <v>856</v>
       </c>
     </row>
-    <row r="244" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A244" t="s">
         <v>852</v>
       </c>
@@ -21467,7 +21468,7 @@
         <v>856</v>
       </c>
     </row>
-    <row r="245" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A245" t="s">
         <v>852</v>
       </c>
@@ -21535,7 +21536,7 @@
         <v>856</v>
       </c>
     </row>
-    <row r="246" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A246" t="s">
         <v>860</v>
       </c>
@@ -21612,7 +21613,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="247" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A247" t="s">
         <v>865</v>
       </c>
@@ -21683,7 +21684,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="248" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A248" t="s">
         <v>870</v>
       </c>
@@ -21751,7 +21752,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="249" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A249" t="s">
         <v>875</v>
       </c>
@@ -21819,7 +21820,7 @@
         <v>879</v>
       </c>
     </row>
-    <row r="250" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A250" t="s">
         <v>880</v>
       </c>
@@ -21887,7 +21888,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="251" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A251" t="s">
         <v>885</v>
       </c>
@@ -21952,7 +21953,7 @@
         <v>889</v>
       </c>
     </row>
-    <row r="252" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A252" t="s">
         <v>885</v>
       </c>
@@ -22017,7 +22018,7 @@
         <v>889</v>
       </c>
     </row>
-    <row r="253" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A253" t="s">
         <v>891</v>
       </c>
@@ -22094,7 +22095,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="254" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A254" t="s">
         <v>896</v>
       </c>
@@ -22171,7 +22172,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="255" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A255" t="s">
         <v>901</v>
       </c>
@@ -22233,7 +22234,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="256" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A256" t="s">
         <v>906</v>
       </c>
@@ -22289,7 +22290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A257" t="s">
         <v>909</v>
       </c>
@@ -22363,7 +22364,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="258" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A258" t="s">
         <v>914</v>
       </c>
@@ -22440,7 +22441,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="259" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A259" t="s">
         <v>919</v>
       </c>
@@ -22508,7 +22509,7 @@
         <v>923</v>
       </c>
     </row>
-    <row r="260" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A260" t="s">
         <v>919</v>
       </c>
@@ -22576,7 +22577,7 @@
         <v>923</v>
       </c>
     </row>
-    <row r="261" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A261" t="s">
         <v>919</v>
       </c>
@@ -22644,7 +22645,7 @@
         <v>923</v>
       </c>
     </row>
-    <row r="262" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A262" t="s">
         <v>926</v>
       </c>
@@ -22700,7 +22701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A263" t="s">
         <v>929</v>
       </c>
@@ -22774,7 +22775,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="264" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A264" t="s">
         <v>934</v>
       </c>
@@ -22839,7 +22840,7 @@
         <v>938</v>
       </c>
     </row>
-    <row r="265" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A265" t="s">
         <v>934</v>
       </c>
@@ -22904,7 +22905,7 @@
         <v>938</v>
       </c>
     </row>
-    <row r="266" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A266" t="s">
         <v>940</v>
       </c>
@@ -22981,7 +22982,7 @@
         <v>944</v>
       </c>
     </row>
-    <row r="267" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A267" t="s">
         <v>945</v>
       </c>
@@ -23037,7 +23038,7 @@
         <v>949</v>
       </c>
     </row>
-    <row r="268" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A268" t="s">
         <v>950</v>
       </c>
@@ -23111,7 +23112,7 @@
         <v>954</v>
       </c>
     </row>
-    <row r="269" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A269" t="s">
         <v>955</v>
       </c>
@@ -23188,7 +23189,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="270" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A270" t="s">
         <v>960</v>
       </c>
@@ -23244,7 +23245,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="271" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A271" t="s">
         <v>965</v>
       </c>
@@ -23315,7 +23316,7 @@
         <v>969</v>
       </c>
     </row>
-    <row r="272" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A272" t="s">
         <v>970</v>
       </c>
@@ -23383,7 +23384,7 @@
         <v>974</v>
       </c>
     </row>
-    <row r="273" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A273" t="s">
         <v>975</v>
       </c>
@@ -23451,7 +23452,7 @@
         <v>979</v>
       </c>
     </row>
-    <row r="274" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A274" t="s">
         <v>980</v>
       </c>
@@ -23516,7 +23517,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="275" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A275" t="s">
         <v>985</v>
       </c>
@@ -23584,7 +23585,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="276" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A276" t="s">
         <v>990</v>
       </c>
@@ -23652,7 +23653,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="277" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A277" t="s">
         <v>995</v>
       </c>
@@ -23720,7 +23721,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="278" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A278" t="s">
         <v>1000</v>
       </c>
@@ -23794,7 +23795,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="279" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A279" t="s">
         <v>1005</v>
       </c>
@@ -23850,7 +23851,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="280" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A280" t="s">
         <v>1005</v>
       </c>
@@ -23906,7 +23907,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="281" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A281" t="s">
         <v>1011</v>
       </c>
@@ -23980,7 +23981,7 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="282" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A282" t="s">
         <v>1016</v>
       </c>
@@ -24048,7 +24049,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="283" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A283" t="s">
         <v>1021</v>
       </c>
@@ -24116,7 +24117,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="284" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A284" t="s">
         <v>1026</v>
       </c>
@@ -24184,7 +24185,7 @@
         <v>1030</v>
       </c>
     </row>
-    <row r="285" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A285" t="s">
         <v>1031</v>
       </c>
@@ -24252,7 +24253,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="286" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A286" t="s">
         <v>1036</v>
       </c>
@@ -24323,7 +24324,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="287" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A287" t="s">
         <v>1041</v>
       </c>
@@ -24388,7 +24389,7 @@
         <v>1045</v>
       </c>
     </row>
-    <row r="288" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A288" t="s">
         <v>1041</v>
       </c>
@@ -24453,7 +24454,7 @@
         <v>1045</v>
       </c>
     </row>
-    <row r="289" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A289" t="s">
         <v>1041</v>
       </c>
@@ -24518,7 +24519,7 @@
         <v>1045</v>
       </c>
     </row>
-    <row r="290" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A290" t="s">
         <v>1041</v>
       </c>
@@ -24583,7 +24584,7 @@
         <v>1045</v>
       </c>
     </row>
-    <row r="291" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A291" t="s">
         <v>1041</v>
       </c>
@@ -24648,7 +24649,7 @@
         <v>1045</v>
       </c>
     </row>
-    <row r="292" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A292" t="s">
         <v>1049</v>
       </c>
@@ -24719,7 +24720,7 @@
         <v>1053</v>
       </c>
     </row>
-    <row r="293" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A293" t="s">
         <v>1049</v>
       </c>
@@ -24790,7 +24791,7 @@
         <v>1053</v>
       </c>
     </row>
-    <row r="294" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A294" t="s">
         <v>1049</v>
       </c>
@@ -24861,7 +24862,7 @@
         <v>1053</v>
       </c>
     </row>
-    <row r="295" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A295" t="s">
         <v>1049</v>
       </c>
@@ -24932,7 +24933,7 @@
         <v>1053</v>
       </c>
     </row>
-    <row r="296" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A296" t="s">
         <v>1049</v>
       </c>
@@ -25003,7 +25004,7 @@
         <v>1053</v>
       </c>
     </row>
-    <row r="297" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A297" t="s">
         <v>1056</v>
       </c>
@@ -25077,7 +25078,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="298" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A298" t="s">
         <v>1061</v>
       </c>
@@ -25142,7 +25143,7 @@
         <v>1065</v>
       </c>
     </row>
-    <row r="299" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A299" t="s">
         <v>1061</v>
       </c>
@@ -25207,7 +25208,7 @@
         <v>1065</v>
       </c>
     </row>
-    <row r="300" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A300" t="s">
         <v>1061</v>
       </c>
@@ -25272,7 +25273,7 @@
         <v>1065</v>
       </c>
     </row>
-    <row r="301" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A301" t="s">
         <v>1061</v>
       </c>
@@ -25337,7 +25338,7 @@
         <v>1065</v>
       </c>
     </row>
-    <row r="302" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A302" t="s">
         <v>1061</v>
       </c>
@@ -25402,7 +25403,7 @@
         <v>1065</v>
       </c>
     </row>
-    <row r="303" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A303" t="s">
         <v>1068</v>
       </c>
@@ -25467,7 +25468,7 @@
         <v>1072</v>
       </c>
     </row>
-    <row r="304" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A304" t="s">
         <v>1068</v>
       </c>
@@ -25532,7 +25533,7 @@
         <v>1072</v>
       </c>
     </row>
-    <row r="305" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A305" t="s">
         <v>1074</v>
       </c>
@@ -25600,7 +25601,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="306" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A306" t="s">
         <v>1079</v>
       </c>
@@ -25656,7 +25657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="307" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A307" t="s">
         <v>1079</v>
       </c>
@@ -25712,7 +25713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="308" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A308" t="s">
         <v>1083</v>
       </c>
@@ -25777,7 +25778,7 @@
         <v>1087</v>
       </c>
     </row>
-    <row r="309" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A309" t="s">
         <v>1088</v>
       </c>
@@ -25845,7 +25846,7 @@
         <v>1092</v>
       </c>
     </row>
-    <row r="310" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A310" t="s">
         <v>1088</v>
       </c>
@@ -25913,7 +25914,7 @@
         <v>1092</v>
       </c>
     </row>
-    <row r="311" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A311" t="s">
         <v>1094</v>
       </c>
@@ -25990,7 +25991,7 @@
         <v>1098</v>
       </c>
     </row>
-    <row r="312" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A312" t="s">
         <v>1099</v>
       </c>
@@ -26058,7 +26059,7 @@
         <v>1103</v>
       </c>
     </row>
-    <row r="313" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A313" t="s">
         <v>1461</v>
       </c>
@@ -26111,7 +26112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="314" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A314" t="s">
         <v>1104</v>
       </c>
@@ -26182,7 +26183,7 @@
         <v>1108</v>
       </c>
     </row>
-    <row r="315" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A315" t="s">
         <v>1104</v>
       </c>
@@ -26253,7 +26254,7 @@
         <v>1108</v>
       </c>
     </row>
-    <row r="316" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A316" t="s">
         <v>1104</v>
       </c>
@@ -26324,7 +26325,7 @@
         <v>1108</v>
       </c>
     </row>
-    <row r="317" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A317" t="s">
         <v>1110</v>
       </c>
@@ -26401,7 +26402,7 @@
         <v>1114</v>
       </c>
     </row>
-    <row r="318" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A318" t="s">
         <v>1115</v>
       </c>
@@ -26469,7 +26470,7 @@
         <v>1119</v>
       </c>
     </row>
-    <row r="319" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A319" t="s">
         <v>1120</v>
       </c>
@@ -26531,7 +26532,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="320" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A320" t="s">
         <v>1120</v>
       </c>
@@ -26593,7 +26594,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="321" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A321" t="s">
         <v>1120</v>
       </c>
@@ -26655,7 +26656,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="322" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A322" t="s">
         <v>1120</v>
       </c>
@@ -26717,7 +26718,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="323" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A323" t="s">
         <v>1120</v>
       </c>
@@ -26779,7 +26780,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="324" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A324" t="s">
         <v>1120</v>
       </c>
@@ -26841,7 +26842,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="325" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A325" t="s">
         <v>1127</v>
       </c>
@@ -26903,7 +26904,7 @@
         <v>1131</v>
       </c>
     </row>
-    <row r="326" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A326" t="s">
         <v>1127</v>
       </c>
@@ -26965,7 +26966,7 @@
         <v>1131</v>
       </c>
     </row>
-    <row r="327" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A327" t="s">
         <v>1127</v>
       </c>
@@ -27027,7 +27028,7 @@
         <v>1131</v>
       </c>
     </row>
-    <row r="328" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A328" t="s">
         <v>1133</v>
       </c>
@@ -27077,7 +27078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="329" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A329" t="s">
         <v>1133</v>
       </c>
@@ -27127,7 +27128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="330" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A330" t="s">
         <v>1136</v>
       </c>
@@ -27195,7 +27196,7 @@
         <v>1140</v>
       </c>
     </row>
-    <row r="331" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A331" t="s">
         <v>1136</v>
       </c>
@@ -27263,7 +27264,7 @@
         <v>1140</v>
       </c>
     </row>
-    <row r="332" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A332" t="s">
         <v>1142</v>
       </c>
@@ -27340,7 +27341,7 @@
         <v>1146</v>
       </c>
     </row>
-    <row r="333" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A333" t="s">
         <v>1147</v>
       </c>
@@ -27414,7 +27415,7 @@
         <v>1151</v>
       </c>
     </row>
-    <row r="334" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A334" t="s">
         <v>1152</v>
       </c>
@@ -27482,7 +27483,7 @@
         <v>1156</v>
       </c>
     </row>
-    <row r="335" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A335" t="s">
         <v>1157</v>
       </c>
@@ -27556,7 +27557,7 @@
         <v>1161</v>
       </c>
     </row>
-    <row r="336" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A336" t="s">
         <v>1162</v>
       </c>
@@ -27612,7 +27613,7 @@
         <v>1166</v>
       </c>
     </row>
-    <row r="337" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A337" t="s">
         <v>1162</v>
       </c>
@@ -27668,7 +27669,7 @@
         <v>1166</v>
       </c>
     </row>
-    <row r="338" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A338" t="s">
         <v>1162</v>
       </c>
@@ -27724,7 +27725,7 @@
         <v>1166</v>
       </c>
     </row>
-    <row r="339" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A339" t="s">
         <v>1169</v>
       </c>
@@ -27792,7 +27793,7 @@
         <v>1173</v>
       </c>
     </row>
-    <row r="340" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A340" t="s">
         <v>1169</v>
       </c>
@@ -27860,7 +27861,7 @@
         <v>1173</v>
       </c>
     </row>
-    <row r="341" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A341" t="s">
         <v>1169</v>
       </c>
@@ -27928,7 +27929,7 @@
         <v>1173</v>
       </c>
     </row>
-    <row r="342" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A342" t="s">
         <v>1175</v>
       </c>
@@ -28002,7 +28003,7 @@
         <v>1179</v>
       </c>
     </row>
-    <row r="343" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A343" t="s">
         <v>1180</v>
       </c>
@@ -28079,7 +28080,7 @@
         <v>1184</v>
       </c>
     </row>
-    <row r="344" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A344" t="s">
         <v>1185</v>
       </c>
@@ -28153,7 +28154,7 @@
         <v>1189</v>
       </c>
     </row>
-    <row r="345" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A345" t="s">
         <v>1190</v>
       </c>
@@ -28224,7 +28225,7 @@
         <v>1194</v>
       </c>
     </row>
-    <row r="346" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A346" t="s">
         <v>1190</v>
       </c>
@@ -28295,7 +28296,7 @@
         <v>1194</v>
       </c>
     </row>
-    <row r="347" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A347" t="s">
         <v>1196</v>
       </c>
@@ -28366,7 +28367,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="348" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A348" t="s">
         <v>1201</v>
       </c>
@@ -28434,7 +28435,7 @@
         <v>1205</v>
       </c>
     </row>
-    <row r="349" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A349" t="s">
         <v>1206</v>
       </c>
@@ -28508,7 +28509,7 @@
         <v>1210</v>
       </c>
     </row>
-    <row r="350" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A350" t="s">
         <v>1206</v>
       </c>
@@ -28582,7 +28583,7 @@
         <v>1210</v>
       </c>
     </row>
-    <row r="351" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A351" t="s">
         <v>1206</v>
       </c>
@@ -28656,7 +28657,7 @@
         <v>1210</v>
       </c>
     </row>
-    <row r="352" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A352" t="s">
         <v>1213</v>
       </c>
@@ -28727,7 +28728,7 @@
         <v>1217</v>
       </c>
     </row>
-    <row r="353" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A353" t="s">
         <v>1213</v>
       </c>
@@ -28798,7 +28799,7 @@
         <v>1217</v>
       </c>
     </row>
-    <row r="354" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A354" t="s">
         <v>1213</v>
       </c>
@@ -28869,7 +28870,7 @@
         <v>1217</v>
       </c>
     </row>
-    <row r="355" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A355" t="s">
         <v>1219</v>
       </c>
@@ -28943,7 +28944,7 @@
         <v>1223</v>
       </c>
     </row>
-    <row r="356" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A356" t="s">
         <v>1224</v>
       </c>
@@ -29011,7 +29012,7 @@
         <v>1228</v>
       </c>
     </row>
-    <row r="357" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A357" t="s">
         <v>1224</v>
       </c>
@@ -29079,7 +29080,7 @@
         <v>1228</v>
       </c>
     </row>
-    <row r="358" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A358" t="s">
         <v>1230</v>
       </c>
@@ -29150,7 +29151,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="359" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A359" t="s">
         <v>1230</v>
       </c>
@@ -29221,7 +29222,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="360" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A360" t="s">
         <v>1230</v>
       </c>
@@ -29292,7 +29293,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="361" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A361" t="s">
         <v>1236</v>
       </c>
@@ -29369,7 +29370,7 @@
         <v>1240</v>
       </c>
     </row>
-    <row r="362" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A362" t="s">
         <v>1241</v>
       </c>
@@ -29446,7 +29447,7 @@
         <v>1245</v>
       </c>
     </row>
-    <row r="363" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A363" t="s">
         <v>1246</v>
       </c>
@@ -29514,7 +29515,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="364" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A364" t="s">
         <v>1251</v>
       </c>
@@ -29582,7 +29583,7 @@
         <v>1255</v>
       </c>
     </row>
-    <row r="365" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A365" t="s">
         <v>1256</v>
       </c>
@@ -29632,7 +29633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="366" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A366" t="s">
         <v>1256</v>
       </c>
@@ -29682,7 +29683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="367" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A367" t="s">
         <v>1260</v>
       </c>
@@ -29750,7 +29751,7 @@
         <v>1264</v>
       </c>
     </row>
-    <row r="368" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A368" t="s">
         <v>1265</v>
       </c>
@@ -29818,7 +29819,7 @@
         <v>1269</v>
       </c>
     </row>
-    <row r="369" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A369" t="s">
         <v>1265</v>
       </c>
@@ -29886,7 +29887,7 @@
         <v>1269</v>
       </c>
     </row>
-    <row r="370" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A370" t="s">
         <v>1265</v>
       </c>
@@ -29954,7 +29955,7 @@
         <v>1269</v>
       </c>
     </row>
-    <row r="371" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A371" t="s">
         <v>1265</v>
       </c>
@@ -30022,7 +30023,7 @@
         <v>1269</v>
       </c>
     </row>
-    <row r="372" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A372" t="s">
         <v>1272</v>
       </c>
@@ -30090,7 +30091,7 @@
         <v>1276</v>
       </c>
     </row>
-    <row r="373" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A373" t="s">
         <v>1277</v>
       </c>
@@ -30164,7 +30165,7 @@
         <v>1281</v>
       </c>
     </row>
-    <row r="374" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A374" t="s">
         <v>1277</v>
       </c>
@@ -30238,7 +30239,7 @@
         <v>1281</v>
       </c>
     </row>
-    <row r="375" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A375" t="s">
         <v>1277</v>
       </c>
@@ -30312,7 +30313,7 @@
         <v>1281</v>
       </c>
     </row>
-    <row r="376" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A376" t="s">
         <v>1282</v>
       </c>
@@ -30380,7 +30381,7 @@
         <v>1286</v>
       </c>
     </row>
-    <row r="377" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A377" t="s">
         <v>1287</v>
       </c>
@@ -30448,7 +30449,7 @@
         <v>1291</v>
       </c>
     </row>
-    <row r="378" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A378" t="s">
         <v>1292</v>
       </c>
@@ -30510,7 +30511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="379" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A379" t="s">
         <v>1295</v>
       </c>
@@ -30551,7 +30552,7 @@
         <v>1299</v>
       </c>
     </row>
-    <row r="380" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A380" t="s">
         <v>1295</v>
       </c>
@@ -30592,7 +30593,7 @@
         <v>1299</v>
       </c>
     </row>
-    <row r="381" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A381" t="s">
         <v>1295</v>
       </c>
@@ -30633,7 +30634,7 @@
         <v>1299</v>
       </c>
     </row>
-    <row r="382" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A382" t="s">
         <v>1295</v>
       </c>
@@ -30674,7 +30675,7 @@
         <v>1299</v>
       </c>
     </row>
-    <row r="383" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A383" t="s">
         <v>1302</v>
       </c>
@@ -30751,7 +30752,7 @@
         <v>1306</v>
       </c>
     </row>
-    <row r="384" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A384" t="s">
         <v>1302</v>
       </c>
@@ -30828,7 +30829,7 @@
         <v>1306</v>
       </c>
     </row>
-    <row r="385" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A385" t="s">
         <v>1302</v>
       </c>
@@ -30905,7 +30906,7 @@
         <v>1306</v>
       </c>
     </row>
-    <row r="386" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A386" t="s">
         <v>1309</v>
       </c>
@@ -30982,7 +30983,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="387" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A387" t="s">
         <v>1314</v>
       </c>
@@ -31050,7 +31051,7 @@
         <v>1318</v>
       </c>
     </row>
-    <row r="388" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A388" t="s">
         <v>1319</v>
       </c>
@@ -31100,7 +31101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="389" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A389" t="s">
         <v>1319</v>
       </c>
@@ -31150,7 +31151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="390" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A390" t="s">
         <v>1319</v>
       </c>
@@ -31200,7 +31201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="391" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A391" t="s">
         <v>1319</v>
       </c>
@@ -31250,7 +31251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="392" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A392" t="s">
         <v>1323</v>
       </c>
@@ -31324,7 +31325,7 @@
         <v>1327</v>
       </c>
     </row>
-    <row r="393" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A393" t="s">
         <v>1328</v>
       </c>
@@ -31392,7 +31393,7 @@
         <v>1332</v>
       </c>
     </row>
-    <row r="394" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A394" t="s">
         <v>1328</v>
       </c>
@@ -31460,7 +31461,7 @@
         <v>1332</v>
       </c>
     </row>
-    <row r="395" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A395" t="s">
         <v>1328</v>
       </c>
@@ -31528,7 +31529,7 @@
         <v>1332</v>
       </c>
     </row>
-    <row r="396" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A396" t="s">
         <v>1334</v>
       </c>
@@ -31596,7 +31597,7 @@
         <v>1338</v>
       </c>
     </row>
-    <row r="397" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A397" t="s">
         <v>1339</v>
       </c>
@@ -31652,7 +31653,7 @@
         <v>1343</v>
       </c>
     </row>
-    <row r="398" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A398" t="s">
         <v>1339</v>
       </c>
@@ -31708,7 +31709,7 @@
         <v>1343</v>
       </c>
     </row>
-    <row r="399" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A399" t="s">
         <v>1339</v>
       </c>
@@ -31764,7 +31765,7 @@
         <v>1343</v>
       </c>
     </row>
-    <row r="400" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A400" t="s">
         <v>1346</v>
       </c>
@@ -31838,7 +31839,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="401" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A401" t="s">
         <v>1346</v>
       </c>
@@ -31912,7 +31913,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="402" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A402" t="s">
         <v>1346</v>
       </c>
@@ -31986,7 +31987,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="403" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A403" t="s">
         <v>1346</v>
       </c>
@@ -32060,7 +32061,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="404" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A404" t="s">
         <v>1346</v>
       </c>
@@ -32134,7 +32135,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="405" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A405" t="s">
         <v>1346</v>
       </c>
@@ -32208,7 +32209,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="406" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A406" t="s">
         <v>1354</v>
       </c>
@@ -32282,7 +32283,7 @@
         <v>1358</v>
       </c>
     </row>
-    <row r="407" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A407" t="s">
         <v>1354</v>
       </c>
@@ -32356,7 +32357,7 @@
         <v>1358</v>
       </c>
     </row>
-    <row r="408" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A408" t="s">
         <v>1354</v>
       </c>
@@ -32430,7 +32431,7 @@
         <v>1358</v>
       </c>
     </row>
-    <row r="409" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A409" t="s">
         <v>1354</v>
       </c>
@@ -32504,7 +32505,7 @@
         <v>1358</v>
       </c>
     </row>
-    <row r="410" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A410" t="s">
         <v>1354</v>
       </c>
@@ -32578,7 +32579,7 @@
         <v>1358</v>
       </c>
     </row>
-    <row r="411" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A411" t="s">
         <v>1363</v>
       </c>
@@ -32649,7 +32650,7 @@
         <v>1367</v>
       </c>
     </row>
-    <row r="412" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A412" t="s">
         <v>1363</v>
       </c>
@@ -32720,7 +32721,7 @@
         <v>1367</v>
       </c>
     </row>
-    <row r="413" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A413" t="s">
         <v>1369</v>
       </c>
@@ -32791,7 +32792,7 @@
         <v>1373</v>
       </c>
     </row>
-    <row r="414" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A414" t="s">
         <v>1369</v>
       </c>
@@ -32862,7 +32863,7 @@
         <v>1373</v>
       </c>
     </row>
-    <row r="415" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A415" t="s">
         <v>1369</v>
       </c>
@@ -32933,7 +32934,7 @@
         <v>1373</v>
       </c>
     </row>
-    <row r="416" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A416" t="s">
         <v>1376</v>
       </c>
@@ -33001,7 +33002,7 @@
         <v>1380</v>
       </c>
     </row>
-    <row r="417" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A417" t="s">
         <v>1376</v>
       </c>
@@ -33069,7 +33070,7 @@
         <v>1380</v>
       </c>
     </row>
-    <row r="418" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A418" t="s">
         <v>1382</v>
       </c>
@@ -33137,7 +33138,7 @@
         <v>1386</v>
       </c>
     </row>
-    <row r="419" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A419" t="s">
         <v>1387</v>
       </c>
@@ -33193,7 +33194,7 @@
         <v>1391</v>
       </c>
     </row>
-    <row r="420" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A420" t="s">
         <v>1387</v>
       </c>
@@ -33249,7 +33250,7 @@
         <v>1391</v>
       </c>
     </row>
-    <row r="421" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A421" t="s">
         <v>1387</v>
       </c>
@@ -33305,7 +33306,7 @@
         <v>1391</v>
       </c>
     </row>
-    <row r="422" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A422" t="s">
         <v>1393</v>
       </c>
@@ -33373,7 +33374,7 @@
         <v>1397</v>
       </c>
     </row>
-    <row r="423" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A423" t="s">
         <v>1398</v>
       </c>
@@ -33441,7 +33442,7 @@
         <v>1402</v>
       </c>
     </row>
-    <row r="424" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A424" t="s">
         <v>1398</v>
       </c>
@@ -33509,7 +33510,7 @@
         <v>1402</v>
       </c>
     </row>
-    <row r="425" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A425" t="s">
         <v>1398</v>
       </c>
@@ -33577,7 +33578,7 @@
         <v>1402</v>
       </c>
     </row>
-    <row r="426" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A426" t="s">
         <v>1405</v>
       </c>
@@ -33651,7 +33652,7 @@
         <v>1409</v>
       </c>
     </row>
-    <row r="427" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A427" t="s">
         <v>1410</v>
       </c>
@@ -33728,7 +33729,7 @@
         <v>1414</v>
       </c>
     </row>
-    <row r="428" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:25" x14ac:dyDescent="0.75">
       <c r="A428" t="s">
         <v>1415</v>
       </c>
@@ -33802,7 +33803,7 @@
         <v>1419</v>
       </c>
     </row>
-    <row r="429" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:25" x14ac:dyDescent="0.75">
       <c r="C429" t="s">
         <v>1420</v>
       </c>
@@ -33853,8 +33854,8 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Y429">
-    <sortState ref="A2:Y428">
+  <autoFilter ref="A1:Y429" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Y428">
       <sortCondition ref="A1:A428"/>
     </sortState>
   </autoFilter>
@@ -33864,14 +33865,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -33897,7 +33898,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -33923,7 +33924,7 @@
         <v>1424</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -33949,7 +33950,7 @@
         <v>1426</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -33975,7 +33976,7 @@
         <v>1428</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>66</v>
       </c>
@@ -33998,7 +33999,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>112</v>
       </c>
@@ -34021,7 +34022,7 @@
         <v>1430</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.75">
       <c r="C7" t="s">
         <v>294</v>
       </c>
@@ -34035,7 +34036,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
         <v>1431</v>
       </c>
@@ -34052,7 +34053,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.75">
       <c r="C9" t="s">
         <v>40</v>
       </c>
@@ -34066,7 +34067,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.75">
       <c r="C10" t="s">
         <v>91</v>
       </c>
@@ -34074,7 +34075,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.75">
       <c r="C11" t="s">
         <v>186</v>
       </c>
@@ -34082,7 +34083,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.75">
       <c r="C12" t="s">
         <v>67</v>
       </c>
@@ -34090,7 +34091,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.75">
       <c r="C13" t="s">
         <v>74</v>
       </c>
@@ -34098,7 +34099,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.75">
       <c r="C14" t="s">
         <v>143</v>
       </c>
@@ -34106,7 +34107,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.75">
       <c r="C15" t="s">
         <v>137</v>
       </c>
@@ -34114,7 +34115,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.75">
       <c r="C16" t="s">
         <v>460</v>
       </c>
@@ -34122,7 +34123,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:4" x14ac:dyDescent="0.75">
       <c r="C17" t="s">
         <v>483</v>
       </c>
@@ -34130,7 +34131,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:4" x14ac:dyDescent="0.75">
       <c r="C18" t="s">
         <v>113</v>
       </c>
@@ -34145,14 +34146,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
         <v>1432</v>
       </c>
@@ -34163,7 +34164,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>1433</v>
       </c>
@@ -34174,7 +34175,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>1434</v>
       </c>
@@ -34185,7 +34186,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>1435</v>
       </c>
@@ -34196,7 +34197,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>1436</v>
       </c>
@@ -34207,17 +34208,17 @@
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.75">
       <c r="C6" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.75">
       <c r="C7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.75">
       <c r="C8" t="s">
         <v>52</v>
       </c>

</xml_diff>

<commit_message>
Add 2-digit ISO for Kosovo
</commit_message>
<xml_diff>
--- a/Codes_Masterlist.xlsx
+++ b/Codes_Masterlist.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alice\Box Sync\PhD\Software\Codes-Masterlist\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\boxsync\alepissier\PhD\Software\Codes-Masterlist\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81AB7DD3-34C6-4868-87C7-1EE26D553217}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31910" yWindow="-90" windowWidth="16980" windowHeight="10080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31905" yWindow="-90" windowWidth="16980" windowHeight="10080"/>
   </bookViews>
   <sheets>
     <sheet name="Codes" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4746" uniqueCount="1490">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4748" uniqueCount="1491">
   <si>
     <t>ISO3166.3</t>
   </si>
@@ -4495,12 +4494,15 @@
   </si>
   <si>
     <t>North Macedonia</t>
+  </si>
+  <si>
+    <t>XK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -4514,6 +4516,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -4834,19 +4837,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y429"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="44.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="22" width="9.1328125" customWidth="1"/>
-    <col min="23" max="23" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="22" width="9.140625" customWidth="1"/>
+    <col min="23" max="23" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4923,7 +4926,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -4994,7 +4997,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -5065,7 +5068,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -5136,7 +5139,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>48</v>
       </c>
@@ -5210,7 +5213,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>58</v>
       </c>
@@ -5272,7 +5275,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>58</v>
       </c>
@@ -5334,7 +5337,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>63</v>
       </c>
@@ -5390,7 +5393,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>71</v>
       </c>
@@ -5458,7 +5461,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>79</v>
       </c>
@@ -5523,7 +5526,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>84</v>
       </c>
@@ -5546,7 +5549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>84</v>
       </c>
@@ -5569,7 +5572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>88</v>
       </c>
@@ -5637,7 +5640,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>88</v>
       </c>
@@ -5705,7 +5708,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>88</v>
       </c>
@@ -5773,7 +5776,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>97</v>
       </c>
@@ -5847,7 +5850,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>103</v>
       </c>
@@ -5915,7 +5918,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>103</v>
       </c>
@@ -5983,7 +5986,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>109</v>
       </c>
@@ -6048,7 +6051,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>117</v>
       </c>
@@ -6089,7 +6092,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>117</v>
       </c>
@@ -6130,7 +6133,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>122</v>
       </c>
@@ -6192,7 +6195,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>122</v>
       </c>
@@ -6254,7 +6257,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>128</v>
       </c>
@@ -6328,7 +6331,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>128</v>
       </c>
@@ -6402,7 +6405,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>128</v>
       </c>
@@ -6476,7 +6479,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>128</v>
       </c>
@@ -6550,7 +6553,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>134</v>
       </c>
@@ -6618,7 +6621,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>140</v>
       </c>
@@ -6689,7 +6692,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>147</v>
       </c>
@@ -6757,7 +6760,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>147</v>
       </c>
@@ -6825,7 +6828,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>153</v>
       </c>
@@ -6902,7 +6905,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>158</v>
       </c>
@@ -6973,7 +6976,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>163</v>
       </c>
@@ -7050,7 +7053,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>169</v>
       </c>
@@ -7106,7 +7109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>169</v>
       </c>
@@ -7162,7 +7165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>169</v>
       </c>
@@ -7218,7 +7221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>169</v>
       </c>
@@ -7274,7 +7277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>169</v>
       </c>
@@ -7330,7 +7333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>173</v>
       </c>
@@ -7407,7 +7410,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>178</v>
       </c>
@@ -7475,7 +7478,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>183</v>
       </c>
@@ -7543,7 +7546,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>189</v>
       </c>
@@ -7611,7 +7614,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>189</v>
       </c>
@@ -7679,7 +7682,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>195</v>
       </c>
@@ -7753,7 +7756,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>195</v>
       </c>
@@ -7827,7 +7830,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>201</v>
       </c>
@@ -7895,7 +7898,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>201</v>
       </c>
@@ -7963,7 +7966,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>207</v>
       </c>
@@ -8025,7 +8028,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>207</v>
       </c>
@@ -8087,7 +8090,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>207</v>
       </c>
@@ -8149,7 +8152,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>212</v>
       </c>
@@ -8217,7 +8220,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="53" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>217</v>
       </c>
@@ -8291,7 +8294,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>223</v>
       </c>
@@ -8356,7 +8359,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>230</v>
       </c>
@@ -8433,7 +8436,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>230</v>
       </c>
@@ -8510,7 +8513,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>236</v>
       </c>
@@ -8584,7 +8587,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="58" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>241</v>
       </c>
@@ -8658,7 +8661,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="59" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>246</v>
       </c>
@@ -8726,7 +8729,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="60" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>246</v>
       </c>
@@ -8794,7 +8797,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="61" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>253</v>
       </c>
@@ -8862,7 +8865,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="62" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>258</v>
       </c>
@@ -8918,7 +8921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="63" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>261</v>
       </c>
@@ -8992,7 +8995,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="64" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="64" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>267</v>
       </c>
@@ -9069,7 +9072,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="65" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="65" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>267</v>
       </c>
@@ -9146,7 +9149,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="66" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="66" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>273</v>
       </c>
@@ -9214,7 +9217,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="67" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="67" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>278</v>
       </c>
@@ -9264,7 +9267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="68" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>278</v>
       </c>
@@ -9314,7 +9317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="69" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>281</v>
       </c>
@@ -9382,7 +9385,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="70" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="70" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>286</v>
       </c>
@@ -9456,7 +9459,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="71" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="71" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>291</v>
       </c>
@@ -9524,7 +9527,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="72" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="72" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>291</v>
       </c>
@@ -9592,7 +9595,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="73" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="73" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>298</v>
       </c>
@@ -9669,7 +9672,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="74" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="74" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>298</v>
       </c>
@@ -9746,7 +9749,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="75" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="75" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>298</v>
       </c>
@@ -9823,7 +9826,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="76" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="76" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>304</v>
       </c>
@@ -9900,7 +9903,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="77" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="77" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>310</v>
       </c>
@@ -9977,7 +9980,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="78" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="78" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>310</v>
       </c>
@@ -10054,7 +10057,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="79" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="79" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>310</v>
       </c>
@@ -10131,7 +10134,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="80" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="80" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>310</v>
       </c>
@@ -10208,7 +10211,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="81" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="81" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>310</v>
       </c>
@@ -10285,7 +10288,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="82" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="82" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>319</v>
       </c>
@@ -10362,7 +10365,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="83" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="83" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>319</v>
       </c>
@@ -10439,7 +10442,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="84" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="84" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>319</v>
       </c>
@@ -10516,7 +10519,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="85" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="85" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>319</v>
       </c>
@@ -10593,7 +10596,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="86" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="86" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>326</v>
       </c>
@@ -10649,7 +10652,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="87" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="87" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>331</v>
       </c>
@@ -10723,7 +10726,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="88" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="88" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>336</v>
       </c>
@@ -10800,7 +10803,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="89" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="89" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>341</v>
       </c>
@@ -10874,7 +10877,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="90" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="90" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>341</v>
       </c>
@@ -10948,7 +10951,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="91" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="91" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>341</v>
       </c>
@@ -11022,7 +11025,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="92" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="92" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>348</v>
       </c>
@@ -11096,7 +11099,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="93" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="93" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>353</v>
       </c>
@@ -11167,7 +11170,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="94" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="94" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>358</v>
       </c>
@@ -11238,7 +11241,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="95" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="95" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>358</v>
       </c>
@@ -11309,7 +11312,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="96" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="96" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>358</v>
       </c>
@@ -11380,7 +11383,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="97" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="97" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>364</v>
       </c>
@@ -11430,7 +11433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="98" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>367</v>
       </c>
@@ -11501,7 +11504,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="99" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="99" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>367</v>
       </c>
@@ -11572,7 +11575,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="100" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="100" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>373</v>
       </c>
@@ -11643,7 +11646,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="101" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="101" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>378</v>
       </c>
@@ -11711,7 +11714,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="102" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="102" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>378</v>
       </c>
@@ -11779,7 +11782,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="103" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="103" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>384</v>
       </c>
@@ -11850,7 +11853,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="104" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="104" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>389</v>
       </c>
@@ -11924,7 +11927,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="105" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="105" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>394</v>
       </c>
@@ -11998,7 +12001,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="106" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="106" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>399</v>
       </c>
@@ -12066,7 +12069,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="107" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="107" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>404</v>
       </c>
@@ -12140,7 +12143,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="108" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="108" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>404</v>
       </c>
@@ -12214,7 +12217,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="109" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="109" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>410</v>
       </c>
@@ -12282,7 +12285,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="110" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="110" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>416</v>
       </c>
@@ -12356,7 +12359,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="111" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="111" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>421</v>
       </c>
@@ -12424,7 +12427,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="112" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="112" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>421</v>
       </c>
@@ -12492,7 +12495,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="113" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="113" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>427</v>
       </c>
@@ -12569,7 +12572,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="114" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="114" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>432</v>
       </c>
@@ -12625,7 +12628,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="115" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="115" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>437</v>
       </c>
@@ -12696,7 +12699,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="116" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="116" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>437</v>
       </c>
@@ -12767,7 +12770,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="117" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="117" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>442</v>
       </c>
@@ -12838,7 +12841,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="118" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="118" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>447</v>
       </c>
@@ -12915,7 +12918,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="119" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="119" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>447</v>
       </c>
@@ -12992,7 +12995,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="120" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="120" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>452</v>
       </c>
@@ -13063,7 +13066,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="121" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="121" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>457</v>
       </c>
@@ -13131,7 +13134,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="122" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="122" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>463</v>
       </c>
@@ -13193,7 +13196,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="123" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="123" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>463</v>
       </c>
@@ -13255,7 +13258,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="124" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="124" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>463</v>
       </c>
@@ -13317,7 +13320,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="125" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="125" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>469</v>
       </c>
@@ -13388,7 +13391,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="126" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="126" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>474</v>
       </c>
@@ -13453,7 +13456,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="127" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="127" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>474</v>
       </c>
@@ -13518,7 +13521,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="128" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="128" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>474</v>
       </c>
@@ -13583,7 +13586,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="129" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="129" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>481</v>
       </c>
@@ -13651,7 +13654,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="130" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="130" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>481</v>
       </c>
@@ -13719,7 +13722,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="131" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="131" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>481</v>
       </c>
@@ -13787,7 +13790,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="132" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="132" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>481</v>
       </c>
@@ -13855,7 +13858,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="133" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="133" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>489</v>
       </c>
@@ -13929,7 +13932,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="134" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="134" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>494</v>
       </c>
@@ -13997,7 +14000,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="135" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="135" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>494</v>
       </c>
@@ -14065,7 +14068,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="136" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="136" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>494</v>
       </c>
@@ -14133,7 +14136,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="137" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="137" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>500</v>
       </c>
@@ -14201,7 +14204,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="138" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="138" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>505</v>
       </c>
@@ -14263,7 +14266,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="139" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="139" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>511</v>
       </c>
@@ -14340,7 +14343,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="140" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="140" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>516</v>
       </c>
@@ -14399,7 +14402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="141" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>519</v>
       </c>
@@ -14476,7 +14479,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="142" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="142" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>524</v>
       </c>
@@ -14532,7 +14535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="143" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>527</v>
       </c>
@@ -14609,7 +14612,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="144" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="144" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>527</v>
       </c>
@@ -14686,7 +14689,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="145" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="145" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>533</v>
       </c>
@@ -14763,7 +14766,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="146" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="146" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>538</v>
       </c>
@@ -14837,7 +14840,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="147" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="147" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>543</v>
       </c>
@@ -14908,7 +14911,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="148" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="148" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>548</v>
       </c>
@@ -14982,7 +14985,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="149" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="149" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>553</v>
       </c>
@@ -15047,7 +15050,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="150" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="150" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>558</v>
       </c>
@@ -15121,7 +15124,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="151" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="151" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>563</v>
       </c>
@@ -15177,7 +15180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="152" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>563</v>
       </c>
@@ -15233,7 +15236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="153" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>567</v>
       </c>
@@ -15298,7 +15301,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="154" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="154" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>572</v>
       </c>
@@ -15375,7 +15378,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="155" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="155" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>577</v>
       </c>
@@ -15443,7 +15446,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="156" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="156" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>577</v>
       </c>
@@ -15511,7 +15514,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="157" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="157" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>577</v>
       </c>
@@ -15579,7 +15582,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="158" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="158" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>577</v>
       </c>
@@ -15647,7 +15650,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="159" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="159" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>577</v>
       </c>
@@ -15715,7 +15718,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="160" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="160" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>577</v>
       </c>
@@ -15783,7 +15786,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="161" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="161" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>577</v>
       </c>
@@ -15851,7 +15854,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="162" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="162" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>587</v>
       </c>
@@ -15907,7 +15910,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="163" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="163" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>587</v>
       </c>
@@ -15963,7 +15966,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="164" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="164" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>587</v>
       </c>
@@ -16019,7 +16022,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="165" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="165" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>592</v>
       </c>
@@ -16096,7 +16099,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="166" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="166" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>597</v>
       </c>
@@ -16164,7 +16167,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="167" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="167" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>602</v>
       </c>
@@ -16241,7 +16244,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="168" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="168" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>607</v>
       </c>
@@ -16309,7 +16312,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="169" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="169" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>612</v>
       </c>
@@ -16377,7 +16380,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="170" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="170" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>617</v>
       </c>
@@ -16442,7 +16445,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="171" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="171" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>622</v>
       </c>
@@ -16510,7 +16513,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="172" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="172" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>627</v>
       </c>
@@ -16572,7 +16575,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="173" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="173" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>627</v>
       </c>
@@ -16634,7 +16637,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="174" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="174" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>632</v>
       </c>
@@ -16705,7 +16708,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="175" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="175" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>637</v>
       </c>
@@ -16773,7 +16776,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="176" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="176" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>637</v>
       </c>
@@ -16841,7 +16844,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="177" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="177" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>637</v>
       </c>
@@ -16909,7 +16912,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="178" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="178" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>637</v>
       </c>
@@ -16977,7 +16980,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="179" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="179" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>645</v>
       </c>
@@ -17045,7 +17048,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="180" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="180" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>650</v>
       </c>
@@ -17113,7 +17116,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="181" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="181" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>655</v>
       </c>
@@ -17181,7 +17184,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="182" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="182" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>660</v>
       </c>
@@ -17252,7 +17255,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="183" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="183" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>665</v>
       </c>
@@ -17326,7 +17329,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="184" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="184" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>670</v>
       </c>
@@ -17388,7 +17391,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="185" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="185" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>675</v>
       </c>
@@ -17456,7 +17459,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="186" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="186" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>680</v>
       </c>
@@ -17524,7 +17527,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="187" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="187" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>685</v>
       </c>
@@ -17592,7 +17595,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="188" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="188" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>691</v>
       </c>
@@ -17666,7 +17669,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="189" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="189" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>696</v>
       </c>
@@ -17734,7 +17737,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="190" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="190" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>696</v>
       </c>
@@ -17802,7 +17805,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="191" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="191" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>702</v>
       </c>
@@ -17870,7 +17873,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="192" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="192" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>707</v>
       </c>
@@ -17938,7 +17941,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="193" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="193" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>712</v>
       </c>
@@ -18012,7 +18015,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="194" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="194" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>712</v>
       </c>
@@ -18086,7 +18089,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="195" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="195" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>712</v>
       </c>
@@ -18160,7 +18163,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="196" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="196" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>712</v>
       </c>
@@ -18234,7 +18237,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="197" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="197" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>718</v>
       </c>
@@ -18302,7 +18305,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="198" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="198" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>718</v>
       </c>
@@ -18370,7 +18373,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="199" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="199" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>718</v>
       </c>
@@ -18438,7 +18441,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="200" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="200" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>718</v>
       </c>
@@ -18506,7 +18509,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="201" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="201" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>718</v>
       </c>
@@ -18574,7 +18577,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="202" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="202" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>718</v>
       </c>
@@ -18642,10 +18645,13 @@
         <v>722</v>
       </c>
     </row>
-    <row r="203" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="203" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>728</v>
       </c>
+      <c r="B203" t="s">
+        <v>1490</v>
+      </c>
       <c r="C203" t="s">
         <v>729</v>
       </c>
@@ -18677,10 +18683,13 @@
         <v>731</v>
       </c>
     </row>
-    <row r="204" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="204" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>728</v>
       </c>
+      <c r="B204" t="s">
+        <v>1490</v>
+      </c>
       <c r="C204" t="s">
         <v>732</v>
       </c>
@@ -18712,7 +18721,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="205" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="205" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>733</v>
       </c>
@@ -18780,7 +18789,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="206" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="206" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>738</v>
       </c>
@@ -18848,7 +18857,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="207" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="207" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>738</v>
       </c>
@@ -18916,7 +18925,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="208" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="208" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>738</v>
       </c>
@@ -18984,7 +18993,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="209" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="209" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>738</v>
       </c>
@@ -19052,7 +19061,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="210" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="210" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>746</v>
       </c>
@@ -19120,7 +19129,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="211" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="211" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>751</v>
       </c>
@@ -19197,7 +19206,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="212" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="212" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>756</v>
       </c>
@@ -19265,7 +19274,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="213" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="213" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>756</v>
       </c>
@@ -19333,7 +19342,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="214" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="214" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>762</v>
       </c>
@@ -19407,7 +19416,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="215" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="215" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>762</v>
       </c>
@@ -19481,7 +19490,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="216" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="216" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>768</v>
       </c>
@@ -19546,7 +19555,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="217" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="217" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>773</v>
       </c>
@@ -19614,7 +19623,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="218" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="218" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>778</v>
       </c>
@@ -19688,7 +19697,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="219" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="219" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>783</v>
       </c>
@@ -19759,7 +19768,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="220" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="220" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>788</v>
       </c>
@@ -19830,7 +19839,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="221" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="221" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>793</v>
       </c>
@@ -19901,7 +19910,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="222" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="222" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>798</v>
       </c>
@@ -19966,7 +19975,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="223" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="223" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>798</v>
       </c>
@@ -20031,7 +20040,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="224" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="224" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>798</v>
       </c>
@@ -20096,7 +20105,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="225" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="225" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>798</v>
       </c>
@@ -20161,7 +20170,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="226" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="226" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>798</v>
       </c>
@@ -20226,7 +20235,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="227" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="227" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>798</v>
       </c>
@@ -20291,7 +20300,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="228" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="228" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>808</v>
       </c>
@@ -20362,7 +20371,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="229" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="229" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>808</v>
       </c>
@@ -20433,7 +20442,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="230" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="230" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>808</v>
       </c>
@@ -20504,7 +20513,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="231" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="231" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>814</v>
       </c>
@@ -20572,7 +20581,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="232" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="232" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>819</v>
       </c>
@@ -20637,7 +20646,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="233" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="233" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>824</v>
       </c>
@@ -20705,7 +20714,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="234" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="234" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>824</v>
       </c>
@@ -20773,7 +20782,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="235" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="235" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>824</v>
       </c>
@@ -20841,7 +20850,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="236" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="236" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>831</v>
       </c>
@@ -20918,7 +20927,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="237" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="237" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>836</v>
       </c>
@@ -20986,7 +20995,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="238" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="238" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>841</v>
       </c>
@@ -21060,7 +21069,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="239" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="239" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>846</v>
       </c>
@@ -21128,7 +21137,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="240" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="240" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>846</v>
       </c>
@@ -21196,7 +21205,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="241" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="241" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>852</v>
       </c>
@@ -21264,7 +21273,7 @@
         <v>856</v>
       </c>
     </row>
-    <row r="242" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="242" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>852</v>
       </c>
@@ -21332,7 +21341,7 @@
         <v>856</v>
       </c>
     </row>
-    <row r="243" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="243" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>852</v>
       </c>
@@ -21400,7 +21409,7 @@
         <v>856</v>
       </c>
     </row>
-    <row r="244" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="244" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>852</v>
       </c>
@@ -21468,7 +21477,7 @@
         <v>856</v>
       </c>
     </row>
-    <row r="245" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="245" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>852</v>
       </c>
@@ -21536,7 +21545,7 @@
         <v>856</v>
       </c>
     </row>
-    <row r="246" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="246" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>860</v>
       </c>
@@ -21613,7 +21622,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="247" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="247" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>865</v>
       </c>
@@ -21684,7 +21693,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="248" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="248" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>870</v>
       </c>
@@ -21752,7 +21761,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="249" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="249" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>875</v>
       </c>
@@ -21820,7 +21829,7 @@
         <v>879</v>
       </c>
     </row>
-    <row r="250" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="250" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>880</v>
       </c>
@@ -21888,7 +21897,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="251" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="251" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>885</v>
       </c>
@@ -21953,7 +21962,7 @@
         <v>889</v>
       </c>
     </row>
-    <row r="252" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="252" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>885</v>
       </c>
@@ -22018,7 +22027,7 @@
         <v>889</v>
       </c>
     </row>
-    <row r="253" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="253" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>891</v>
       </c>
@@ -22095,7 +22104,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="254" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="254" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>896</v>
       </c>
@@ -22172,7 +22181,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="255" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="255" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>901</v>
       </c>
@@ -22234,7 +22243,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="256" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="256" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>906</v>
       </c>
@@ -22290,7 +22299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="257" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>909</v>
       </c>
@@ -22364,7 +22373,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="258" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="258" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>914</v>
       </c>
@@ -22441,7 +22450,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="259" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="259" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>919</v>
       </c>
@@ -22509,7 +22518,7 @@
         <v>923</v>
       </c>
     </row>
-    <row r="260" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="260" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>919</v>
       </c>
@@ -22577,7 +22586,7 @@
         <v>923</v>
       </c>
     </row>
-    <row r="261" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="261" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>919</v>
       </c>
@@ -22645,7 +22654,7 @@
         <v>923</v>
       </c>
     </row>
-    <row r="262" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="262" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>926</v>
       </c>
@@ -22701,7 +22710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="263" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>929</v>
       </c>
@@ -22775,7 +22784,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="264" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="264" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>934</v>
       </c>
@@ -22840,7 +22849,7 @@
         <v>938</v>
       </c>
     </row>
-    <row r="265" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="265" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>934</v>
       </c>
@@ -22905,7 +22914,7 @@
         <v>938</v>
       </c>
     </row>
-    <row r="266" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="266" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>940</v>
       </c>
@@ -22982,7 +22991,7 @@
         <v>944</v>
       </c>
     </row>
-    <row r="267" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="267" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>945</v>
       </c>
@@ -23038,7 +23047,7 @@
         <v>949</v>
       </c>
     </row>
-    <row r="268" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="268" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>950</v>
       </c>
@@ -23112,7 +23121,7 @@
         <v>954</v>
       </c>
     </row>
-    <row r="269" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="269" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>955</v>
       </c>
@@ -23189,7 +23198,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="270" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="270" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>960</v>
       </c>
@@ -23245,7 +23254,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="271" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="271" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>965</v>
       </c>
@@ -23316,7 +23325,7 @@
         <v>969</v>
       </c>
     </row>
-    <row r="272" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="272" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>970</v>
       </c>
@@ -23384,7 +23393,7 @@
         <v>974</v>
       </c>
     </row>
-    <row r="273" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="273" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>975</v>
       </c>
@@ -23452,7 +23461,7 @@
         <v>979</v>
       </c>
     </row>
-    <row r="274" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="274" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>980</v>
       </c>
@@ -23517,7 +23526,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="275" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="275" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>985</v>
       </c>
@@ -23585,7 +23594,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="276" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="276" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>990</v>
       </c>
@@ -23653,7 +23662,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="277" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="277" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>995</v>
       </c>
@@ -23721,7 +23730,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="278" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="278" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>1000</v>
       </c>
@@ -23795,7 +23804,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="279" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="279" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>1005</v>
       </c>
@@ -23851,7 +23860,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="280" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="280" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>1005</v>
       </c>
@@ -23907,7 +23916,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="281" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="281" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>1011</v>
       </c>
@@ -23981,7 +23990,7 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="282" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="282" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>1016</v>
       </c>
@@ -24049,7 +24058,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="283" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="283" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>1021</v>
       </c>
@@ -24117,7 +24126,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="284" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="284" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>1026</v>
       </c>
@@ -24185,7 +24194,7 @@
         <v>1030</v>
       </c>
     </row>
-    <row r="285" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="285" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>1031</v>
       </c>
@@ -24253,7 +24262,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="286" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="286" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>1036</v>
       </c>
@@ -24324,7 +24333,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="287" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="287" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>1041</v>
       </c>
@@ -24389,7 +24398,7 @@
         <v>1045</v>
       </c>
     </row>
-    <row r="288" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="288" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>1041</v>
       </c>
@@ -24454,7 +24463,7 @@
         <v>1045</v>
       </c>
     </row>
-    <row r="289" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="289" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>1041</v>
       </c>
@@ -24519,7 +24528,7 @@
         <v>1045</v>
       </c>
     </row>
-    <row r="290" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="290" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>1041</v>
       </c>
@@ -24584,7 +24593,7 @@
         <v>1045</v>
       </c>
     </row>
-    <row r="291" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="291" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>1041</v>
       </c>
@@ -24649,7 +24658,7 @@
         <v>1045</v>
       </c>
     </row>
-    <row r="292" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="292" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>1049</v>
       </c>
@@ -24720,7 +24729,7 @@
         <v>1053</v>
       </c>
     </row>
-    <row r="293" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="293" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>1049</v>
       </c>
@@ -24791,7 +24800,7 @@
         <v>1053</v>
       </c>
     </row>
-    <row r="294" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="294" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>1049</v>
       </c>
@@ -24862,7 +24871,7 @@
         <v>1053</v>
       </c>
     </row>
-    <row r="295" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="295" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>1049</v>
       </c>
@@ -24933,7 +24942,7 @@
         <v>1053</v>
       </c>
     </row>
-    <row r="296" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="296" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>1049</v>
       </c>
@@ -25004,7 +25013,7 @@
         <v>1053</v>
       </c>
     </row>
-    <row r="297" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="297" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>1056</v>
       </c>
@@ -25078,7 +25087,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="298" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="298" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>1061</v>
       </c>
@@ -25143,7 +25152,7 @@
         <v>1065</v>
       </c>
     </row>
-    <row r="299" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="299" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>1061</v>
       </c>
@@ -25208,7 +25217,7 @@
         <v>1065</v>
       </c>
     </row>
-    <row r="300" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="300" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>1061</v>
       </c>
@@ -25273,7 +25282,7 @@
         <v>1065</v>
       </c>
     </row>
-    <row r="301" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="301" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>1061</v>
       </c>
@@ -25338,7 +25347,7 @@
         <v>1065</v>
       </c>
     </row>
-    <row r="302" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="302" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>1061</v>
       </c>
@@ -25403,7 +25412,7 @@
         <v>1065</v>
       </c>
     </row>
-    <row r="303" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="303" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>1068</v>
       </c>
@@ -25468,7 +25477,7 @@
         <v>1072</v>
       </c>
     </row>
-    <row r="304" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="304" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>1068</v>
       </c>
@@ -25533,7 +25542,7 @@
         <v>1072</v>
       </c>
     </row>
-    <row r="305" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="305" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>1074</v>
       </c>
@@ -25601,7 +25610,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="306" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="306" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>1079</v>
       </c>
@@ -25657,7 +25666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="307" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="307" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>1079</v>
       </c>
@@ -25713,7 +25722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="308" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="308" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>1083</v>
       </c>
@@ -25778,7 +25787,7 @@
         <v>1087</v>
       </c>
     </row>
-    <row r="309" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="309" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>1088</v>
       </c>
@@ -25846,7 +25855,7 @@
         <v>1092</v>
       </c>
     </row>
-    <row r="310" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="310" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>1088</v>
       </c>
@@ -25914,7 +25923,7 @@
         <v>1092</v>
       </c>
     </row>
-    <row r="311" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="311" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>1094</v>
       </c>
@@ -25991,7 +26000,7 @@
         <v>1098</v>
       </c>
     </row>
-    <row r="312" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="312" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>1099</v>
       </c>
@@ -26059,7 +26068,7 @@
         <v>1103</v>
       </c>
     </row>
-    <row r="313" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="313" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>1461</v>
       </c>
@@ -26112,7 +26121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="314" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="314" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>1104</v>
       </c>
@@ -26183,7 +26192,7 @@
         <v>1108</v>
       </c>
     </row>
-    <row r="315" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="315" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>1104</v>
       </c>
@@ -26254,7 +26263,7 @@
         <v>1108</v>
       </c>
     </row>
-    <row r="316" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="316" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>1104</v>
       </c>
@@ -26325,7 +26334,7 @@
         <v>1108</v>
       </c>
     </row>
-    <row r="317" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="317" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>1110</v>
       </c>
@@ -26402,7 +26411,7 @@
         <v>1114</v>
       </c>
     </row>
-    <row r="318" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="318" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>1115</v>
       </c>
@@ -26470,7 +26479,7 @@
         <v>1119</v>
       </c>
     </row>
-    <row r="319" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="319" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>1120</v>
       </c>
@@ -26532,7 +26541,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="320" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="320" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>1120</v>
       </c>
@@ -26594,7 +26603,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="321" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="321" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>1120</v>
       </c>
@@ -26656,7 +26665,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="322" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="322" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>1120</v>
       </c>
@@ -26718,7 +26727,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="323" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="323" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>1120</v>
       </c>
@@ -26780,7 +26789,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="324" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="324" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
         <v>1120</v>
       </c>
@@ -26842,7 +26851,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="325" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="325" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
         <v>1127</v>
       </c>
@@ -26904,7 +26913,7 @@
         <v>1131</v>
       </c>
     </row>
-    <row r="326" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="326" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
         <v>1127</v>
       </c>
@@ -26966,7 +26975,7 @@
         <v>1131</v>
       </c>
     </row>
-    <row r="327" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="327" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>1127</v>
       </c>
@@ -27028,7 +27037,7 @@
         <v>1131</v>
       </c>
     </row>
-    <row r="328" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="328" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>1133</v>
       </c>
@@ -27078,7 +27087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="329" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="329" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>1133</v>
       </c>
@@ -27128,7 +27137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="330" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="330" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>1136</v>
       </c>
@@ -27196,7 +27205,7 @@
         <v>1140</v>
       </c>
     </row>
-    <row r="331" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="331" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>1136</v>
       </c>
@@ -27264,7 +27273,7 @@
         <v>1140</v>
       </c>
     </row>
-    <row r="332" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="332" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
         <v>1142</v>
       </c>
@@ -27341,7 +27350,7 @@
         <v>1146</v>
       </c>
     </row>
-    <row r="333" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="333" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>1147</v>
       </c>
@@ -27415,7 +27424,7 @@
         <v>1151</v>
       </c>
     </row>
-    <row r="334" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="334" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
         <v>1152</v>
       </c>
@@ -27483,7 +27492,7 @@
         <v>1156</v>
       </c>
     </row>
-    <row r="335" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="335" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
         <v>1157</v>
       </c>
@@ -27557,7 +27566,7 @@
         <v>1161</v>
       </c>
     </row>
-    <row r="336" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="336" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
         <v>1162</v>
       </c>
@@ -27613,7 +27622,7 @@
         <v>1166</v>
       </c>
     </row>
-    <row r="337" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="337" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
         <v>1162</v>
       </c>
@@ -27669,7 +27678,7 @@
         <v>1166</v>
       </c>
     </row>
-    <row r="338" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="338" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>1162</v>
       </c>
@@ -27725,7 +27734,7 @@
         <v>1166</v>
       </c>
     </row>
-    <row r="339" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="339" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>1169</v>
       </c>
@@ -27793,7 +27802,7 @@
         <v>1173</v>
       </c>
     </row>
-    <row r="340" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="340" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
         <v>1169</v>
       </c>
@@ -27861,7 +27870,7 @@
         <v>1173</v>
       </c>
     </row>
-    <row r="341" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="341" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
         <v>1169</v>
       </c>
@@ -27929,7 +27938,7 @@
         <v>1173</v>
       </c>
     </row>
-    <row r="342" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="342" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
         <v>1175</v>
       </c>
@@ -28003,7 +28012,7 @@
         <v>1179</v>
       </c>
     </row>
-    <row r="343" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="343" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
         <v>1180</v>
       </c>
@@ -28080,7 +28089,7 @@
         <v>1184</v>
       </c>
     </row>
-    <row r="344" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="344" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
         <v>1185</v>
       </c>
@@ -28154,7 +28163,7 @@
         <v>1189</v>
       </c>
     </row>
-    <row r="345" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="345" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
         <v>1190</v>
       </c>
@@ -28225,7 +28234,7 @@
         <v>1194</v>
       </c>
     </row>
-    <row r="346" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="346" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>1190</v>
       </c>
@@ -28296,7 +28305,7 @@
         <v>1194</v>
       </c>
     </row>
-    <row r="347" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="347" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
         <v>1196</v>
       </c>
@@ -28367,7 +28376,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="348" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="348" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
         <v>1201</v>
       </c>
@@ -28435,7 +28444,7 @@
         <v>1205</v>
       </c>
     </row>
-    <row r="349" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="349" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
         <v>1206</v>
       </c>
@@ -28509,7 +28518,7 @@
         <v>1210</v>
       </c>
     </row>
-    <row r="350" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="350" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>1206</v>
       </c>
@@ -28583,7 +28592,7 @@
         <v>1210</v>
       </c>
     </row>
-    <row r="351" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="351" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
         <v>1206</v>
       </c>
@@ -28657,7 +28666,7 @@
         <v>1210</v>
       </c>
     </row>
-    <row r="352" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="352" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
         <v>1213</v>
       </c>
@@ -28728,7 +28737,7 @@
         <v>1217</v>
       </c>
     </row>
-    <row r="353" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="353" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
         <v>1213</v>
       </c>
@@ -28799,7 +28808,7 @@
         <v>1217</v>
       </c>
     </row>
-    <row r="354" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="354" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
         <v>1213</v>
       </c>
@@ -28870,7 +28879,7 @@
         <v>1217</v>
       </c>
     </row>
-    <row r="355" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="355" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
         <v>1219</v>
       </c>
@@ -28944,7 +28953,7 @@
         <v>1223</v>
       </c>
     </row>
-    <row r="356" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="356" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
         <v>1224</v>
       </c>
@@ -29012,7 +29021,7 @@
         <v>1228</v>
       </c>
     </row>
-    <row r="357" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="357" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
         <v>1224</v>
       </c>
@@ -29080,7 +29089,7 @@
         <v>1228</v>
       </c>
     </row>
-    <row r="358" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="358" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
         <v>1230</v>
       </c>
@@ -29151,7 +29160,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="359" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="359" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
         <v>1230</v>
       </c>
@@ -29222,7 +29231,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="360" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="360" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
         <v>1230</v>
       </c>
@@ -29293,7 +29302,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="361" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="361" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
         <v>1236</v>
       </c>
@@ -29370,7 +29379,7 @@
         <v>1240</v>
       </c>
     </row>
-    <row r="362" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="362" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
         <v>1241</v>
       </c>
@@ -29447,7 +29456,7 @@
         <v>1245</v>
       </c>
     </row>
-    <row r="363" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="363" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
         <v>1246</v>
       </c>
@@ -29515,7 +29524,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="364" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="364" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
         <v>1251</v>
       </c>
@@ -29583,7 +29592,7 @@
         <v>1255</v>
       </c>
     </row>
-    <row r="365" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="365" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
         <v>1256</v>
       </c>
@@ -29633,7 +29642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="366" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="366" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
         <v>1256</v>
       </c>
@@ -29683,7 +29692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="367" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="367" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
         <v>1260</v>
       </c>
@@ -29751,7 +29760,7 @@
         <v>1264</v>
       </c>
     </row>
-    <row r="368" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="368" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
         <v>1265</v>
       </c>
@@ -29819,7 +29828,7 @@
         <v>1269</v>
       </c>
     </row>
-    <row r="369" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="369" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
         <v>1265</v>
       </c>
@@ -29887,7 +29896,7 @@
         <v>1269</v>
       </c>
     </row>
-    <row r="370" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="370" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
         <v>1265</v>
       </c>
@@ -29955,7 +29964,7 @@
         <v>1269</v>
       </c>
     </row>
-    <row r="371" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="371" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
         <v>1265</v>
       </c>
@@ -30023,7 +30032,7 @@
         <v>1269</v>
       </c>
     </row>
-    <row r="372" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="372" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
         <v>1272</v>
       </c>
@@ -30091,7 +30100,7 @@
         <v>1276</v>
       </c>
     </row>
-    <row r="373" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="373" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
         <v>1277</v>
       </c>
@@ -30165,7 +30174,7 @@
         <v>1281</v>
       </c>
     </row>
-    <row r="374" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="374" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
         <v>1277</v>
       </c>
@@ -30239,7 +30248,7 @@
         <v>1281</v>
       </c>
     </row>
-    <row r="375" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="375" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
         <v>1277</v>
       </c>
@@ -30313,7 +30322,7 @@
         <v>1281</v>
       </c>
     </row>
-    <row r="376" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="376" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
         <v>1282</v>
       </c>
@@ -30381,7 +30390,7 @@
         <v>1286</v>
       </c>
     </row>
-    <row r="377" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="377" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
         <v>1287</v>
       </c>
@@ -30449,7 +30458,7 @@
         <v>1291</v>
       </c>
     </row>
-    <row r="378" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="378" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
         <v>1292</v>
       </c>
@@ -30511,7 +30520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="379" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="379" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
         <v>1295</v>
       </c>
@@ -30552,7 +30561,7 @@
         <v>1299</v>
       </c>
     </row>
-    <row r="380" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="380" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
         <v>1295</v>
       </c>
@@ -30593,7 +30602,7 @@
         <v>1299</v>
       </c>
     </row>
-    <row r="381" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="381" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
         <v>1295</v>
       </c>
@@ -30634,7 +30643,7 @@
         <v>1299</v>
       </c>
     </row>
-    <row r="382" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="382" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
         <v>1295</v>
       </c>
@@ -30675,7 +30684,7 @@
         <v>1299</v>
       </c>
     </row>
-    <row r="383" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="383" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
         <v>1302</v>
       </c>
@@ -30752,7 +30761,7 @@
         <v>1306</v>
       </c>
     </row>
-    <row r="384" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="384" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
         <v>1302</v>
       </c>
@@ -30829,7 +30838,7 @@
         <v>1306</v>
       </c>
     </row>
-    <row r="385" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="385" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
         <v>1302</v>
       </c>
@@ -30906,7 +30915,7 @@
         <v>1306</v>
       </c>
     </row>
-    <row r="386" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="386" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
         <v>1309</v>
       </c>
@@ -30983,7 +30992,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="387" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="387" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
         <v>1314</v>
       </c>
@@ -31051,7 +31060,7 @@
         <v>1318</v>
       </c>
     </row>
-    <row r="388" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="388" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
         <v>1319</v>
       </c>
@@ -31101,7 +31110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="389" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="389" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
         <v>1319</v>
       </c>
@@ -31151,7 +31160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="390" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="390" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
         <v>1319</v>
       </c>
@@ -31201,7 +31210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="391" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="391" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
         <v>1319</v>
       </c>
@@ -31251,7 +31260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="392" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="392" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
         <v>1323</v>
       </c>
@@ -31325,7 +31334,7 @@
         <v>1327</v>
       </c>
     </row>
-    <row r="393" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="393" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
         <v>1328</v>
       </c>
@@ -31393,7 +31402,7 @@
         <v>1332</v>
       </c>
     </row>
-    <row r="394" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="394" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
         <v>1328</v>
       </c>
@@ -31461,7 +31470,7 @@
         <v>1332</v>
       </c>
     </row>
-    <row r="395" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="395" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
         <v>1328</v>
       </c>
@@ -31529,7 +31538,7 @@
         <v>1332</v>
       </c>
     </row>
-    <row r="396" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="396" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
         <v>1334</v>
       </c>
@@ -31597,7 +31606,7 @@
         <v>1338</v>
       </c>
     </row>
-    <row r="397" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="397" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
         <v>1339</v>
       </c>
@@ -31653,7 +31662,7 @@
         <v>1343</v>
       </c>
     </row>
-    <row r="398" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="398" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
         <v>1339</v>
       </c>
@@ -31709,7 +31718,7 @@
         <v>1343</v>
       </c>
     </row>
-    <row r="399" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="399" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
         <v>1339</v>
       </c>
@@ -31765,7 +31774,7 @@
         <v>1343</v>
       </c>
     </row>
-    <row r="400" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="400" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
         <v>1346</v>
       </c>
@@ -31839,7 +31848,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="401" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="401" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
         <v>1346</v>
       </c>
@@ -31913,7 +31922,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="402" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="402" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
         <v>1346</v>
       </c>
@@ -31987,7 +31996,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="403" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="403" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
         <v>1346</v>
       </c>
@@ -32061,7 +32070,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="404" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="404" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
         <v>1346</v>
       </c>
@@ -32135,7 +32144,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="405" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="405" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
         <v>1346</v>
       </c>
@@ -32209,7 +32218,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="406" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="406" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
         <v>1354</v>
       </c>
@@ -32283,7 +32292,7 @@
         <v>1358</v>
       </c>
     </row>
-    <row r="407" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="407" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
         <v>1354</v>
       </c>
@@ -32357,7 +32366,7 @@
         <v>1358</v>
       </c>
     </row>
-    <row r="408" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="408" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
         <v>1354</v>
       </c>
@@ -32431,7 +32440,7 @@
         <v>1358</v>
       </c>
     </row>
-    <row r="409" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="409" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
         <v>1354</v>
       </c>
@@ -32505,7 +32514,7 @@
         <v>1358</v>
       </c>
     </row>
-    <row r="410" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="410" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
         <v>1354</v>
       </c>
@@ -32579,7 +32588,7 @@
         <v>1358</v>
       </c>
     </row>
-    <row r="411" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="411" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
         <v>1363</v>
       </c>
@@ -32650,7 +32659,7 @@
         <v>1367</v>
       </c>
     </row>
-    <row r="412" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="412" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
         <v>1363</v>
       </c>
@@ -32721,7 +32730,7 @@
         <v>1367</v>
       </c>
     </row>
-    <row r="413" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="413" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
         <v>1369</v>
       </c>
@@ -32792,7 +32801,7 @@
         <v>1373</v>
       </c>
     </row>
-    <row r="414" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="414" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
         <v>1369</v>
       </c>
@@ -32863,7 +32872,7 @@
         <v>1373</v>
       </c>
     </row>
-    <row r="415" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="415" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
         <v>1369</v>
       </c>
@@ -32934,7 +32943,7 @@
         <v>1373</v>
       </c>
     </row>
-    <row r="416" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="416" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
         <v>1376</v>
       </c>
@@ -33002,7 +33011,7 @@
         <v>1380</v>
       </c>
     </row>
-    <row r="417" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="417" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
         <v>1376</v>
       </c>
@@ -33070,7 +33079,7 @@
         <v>1380</v>
       </c>
     </row>
-    <row r="418" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="418" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
         <v>1382</v>
       </c>
@@ -33138,7 +33147,7 @@
         <v>1386</v>
       </c>
     </row>
-    <row r="419" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="419" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
         <v>1387</v>
       </c>
@@ -33194,7 +33203,7 @@
         <v>1391</v>
       </c>
     </row>
-    <row r="420" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="420" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
         <v>1387</v>
       </c>
@@ -33250,7 +33259,7 @@
         <v>1391</v>
       </c>
     </row>
-    <row r="421" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="421" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
         <v>1387</v>
       </c>
@@ -33306,7 +33315,7 @@
         <v>1391</v>
       </c>
     </row>
-    <row r="422" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="422" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
         <v>1393</v>
       </c>
@@ -33374,7 +33383,7 @@
         <v>1397</v>
       </c>
     </row>
-    <row r="423" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="423" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
         <v>1398</v>
       </c>
@@ -33442,7 +33451,7 @@
         <v>1402</v>
       </c>
     </row>
-    <row r="424" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="424" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
         <v>1398</v>
       </c>
@@ -33510,7 +33519,7 @@
         <v>1402</v>
       </c>
     </row>
-    <row r="425" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="425" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
         <v>1398</v>
       </c>
@@ -33578,7 +33587,7 @@
         <v>1402</v>
       </c>
     </row>
-    <row r="426" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="426" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
         <v>1405</v>
       </c>
@@ -33652,7 +33661,7 @@
         <v>1409</v>
       </c>
     </row>
-    <row r="427" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="427" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
         <v>1410</v>
       </c>
@@ -33729,7 +33738,7 @@
         <v>1414</v>
       </c>
     </row>
-    <row r="428" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="428" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
         <v>1415</v>
       </c>
@@ -33803,7 +33812,7 @@
         <v>1419</v>
       </c>
     </row>
-    <row r="429" spans="1:25" x14ac:dyDescent="0.75">
+    <row r="429" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C429" t="s">
         <v>1420</v>
       </c>
@@ -33854,8 +33863,8 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Y429" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Y428">
+  <autoFilter ref="A1:Y429">
+    <sortState ref="A2:Y428">
       <sortCondition ref="A1:A428"/>
     </sortState>
   </autoFilter>
@@ -33865,14 +33874,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -33898,7 +33907,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -33924,7 +33933,7 @@
         <v>1424</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -33950,7 +33959,7 @@
         <v>1426</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -33976,7 +33985,7 @@
         <v>1428</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>66</v>
       </c>
@@ -33999,7 +34008,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>112</v>
       </c>
@@ -34022,7 +34031,7 @@
         <v>1430</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>294</v>
       </c>
@@ -34036,7 +34045,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1431</v>
       </c>
@@ -34053,7 +34062,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>40</v>
       </c>
@@ -34067,7 +34076,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>91</v>
       </c>
@@ -34075,7 +34084,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>186</v>
       </c>
@@ -34083,7 +34092,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>67</v>
       </c>
@@ -34091,7 +34100,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>74</v>
       </c>
@@ -34099,7 +34108,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>143</v>
       </c>
@@ -34107,7 +34116,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>137</v>
       </c>
@@ -34115,7 +34124,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>460</v>
       </c>
@@ -34123,7 +34132,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.75">
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>483</v>
       </c>
@@ -34131,7 +34140,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.75">
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>113</v>
       </c>
@@ -34146,14 +34155,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1432</v>
       </c>
@@ -34164,7 +34173,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1433</v>
       </c>
@@ -34175,7 +34184,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1434</v>
       </c>
@@ -34186,7 +34195,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1435</v>
       </c>
@@ -34197,7 +34206,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1436</v>
       </c>
@@ -34208,17 +34217,17 @@
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>52</v>
       </c>

</xml_diff>